<commit_message>
added 2h Tsys measurement
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6556D533-F16A-FE42-87A8-823B55824901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58441F2F-390A-F748-840E-E88B0ADD492B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69800" yWindow="460" windowWidth="35840" windowHeight="19760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65760" yWindow="460" windowWidth="35840" windowHeight="19760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="466">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -840,12 +840,6 @@
   </si>
   <si>
     <t>sn0082A</t>
-  </si>
-  <si>
-    <t>sn0024A</t>
-  </si>
-  <si>
-    <t>sn0073A</t>
   </si>
   <si>
     <t>PAX Box Number</t>
@@ -1733,14 +1727,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -2188,11 +2182,10 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2206,14 +2199,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2237,6 +2230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2480,25 +2474,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="138"/>
-      <c r="Q1" s="138"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="137"/>
+      <c r="P1" s="137"/>
+      <c r="Q1" s="137"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2826,7 +2820,7 @@
         <v>2A</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>53</v>
@@ -2946,7 +2940,7 @@
         <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>68</v>
@@ -3022,7 +3016,7 @@
         <v>2H</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>76</v>
@@ -3059,7 +3053,7 @@
         <v>81</v>
       </c>
       <c r="D21" s="88" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E21" s="84" t="s">
         <v>130</v>
@@ -3138,10 +3132,10 @@
         <v>90</v>
       </c>
       <c r="D24" s="88" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E24" s="87" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F24" s="84"/>
       <c r="G24" s="9"/>
@@ -3796,38 +3790,38 @@
       <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="139" t="s">
+      <c r="A59" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="134"/>
-      <c r="C59" s="134"/>
+      <c r="B59" s="133"/>
+      <c r="C59" s="133"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="133" t="s">
+      <c r="A61" s="132" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="134"/>
-      <c r="C61" s="133" t="s">
+      <c r="B61" s="133"/>
+      <c r="C61" s="132" t="s">
         <v>158</v>
       </c>
-      <c r="D61" s="134"/>
-      <c r="E61" s="134"/>
-      <c r="F61" s="134"/>
+      <c r="D61" s="133"/>
+      <c r="E61" s="133"/>
+      <c r="F61" s="133"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="133" t="s">
+      <c r="A62" s="132" t="s">
         <v>159</v>
       </c>
-      <c r="B62" s="134"/>
-      <c r="C62" s="133" t="s">
+      <c r="B62" s="133"/>
+      <c r="C62" s="132" t="s">
         <v>160</v>
       </c>
-      <c r="D62" s="134"/>
-      <c r="E62" s="134"/>
-      <c r="F62" s="134"/>
+      <c r="D62" s="133"/>
+      <c r="E62" s="133"/>
+      <c r="F62" s="133"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4795,7 +4789,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection sqref="A1:J22"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4808,64 +4802,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="139" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="142" t="s">
+      <c r="B1" s="140"/>
+      <c r="C1" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
       <c r="K1" s="79"/>
       <c r="L1" s="79"/>
     </row>
     <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="128" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="129" t="s">
+      <c r="C2" s="128" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="130" t="s">
+      <c r="D2" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="129" t="s">
+      <c r="E2" s="128" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="129" t="s">
+      <c r="F2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="129" t="s">
+      <c r="G2" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="129" t="s">
+      <c r="H2" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="131" t="s">
+      <c r="J2" s="130" t="s">
         <v>164</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="115" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B3" s="82" t="s">
         <v>165</v>
@@ -4957,7 +4951,7 @@
         <v>5C4-004</v>
       </c>
       <c r="B6" s="75" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>28</v>
@@ -4984,10 +4978,10 @@
         <v>28</v>
       </c>
       <c r="K6" s="74" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L6" s="74" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5023,7 +5017,7 @@
         <v>175</v>
       </c>
       <c r="K7" s="100" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L7" s="74"/>
     </row>
@@ -5060,7 +5054,7 @@
         <v>28</v>
       </c>
       <c r="K8" s="74" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L8" s="74"/>
     </row>
@@ -5069,7 +5063,7 @@
         <v>169</v>
       </c>
       <c r="B9" s="81" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>28</v>
@@ -5096,7 +5090,7 @@
         <v>28</v>
       </c>
       <c r="K9" s="74" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L9" s="74"/>
     </row>
@@ -5106,7 +5100,7 @@
         <v>5C4-008</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>28</v>
@@ -5133,10 +5127,10 @@
         <v>28</v>
       </c>
       <c r="K10" s="74" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L10" s="74" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5180,7 +5174,7 @@
         <v>5C4-010</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>28</v>
@@ -5207,7 +5201,7 @@
         <v>28</v>
       </c>
       <c r="K12" s="74" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L12" s="74"/>
     </row>
@@ -5217,7 +5211,7 @@
         <v>5C4-011</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>28</v>
@@ -5244,10 +5238,10 @@
         <v>28</v>
       </c>
       <c r="K13" s="74" t="s">
+        <v>394</v>
+      </c>
+      <c r="L13" s="74" t="s">
         <v>396</v>
-      </c>
-      <c r="L13" s="74" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5279,11 +5273,11 @@
       <c r="I14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="132" t="s">
+      <c r="J14" s="131" t="s">
         <v>175</v>
       </c>
       <c r="K14" s="100" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="L14" s="74"/>
     </row>
@@ -5293,7 +5287,7 @@
         <v>5C4-013</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>28</v>
@@ -5320,7 +5314,7 @@
         <v>28</v>
       </c>
       <c r="K15" s="74" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="L15" s="74"/>
     </row>
@@ -5330,7 +5324,7 @@
         <v>5C4-014</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>28</v>
@@ -5357,10 +5351,10 @@
         <v>28</v>
       </c>
       <c r="K16" s="74" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L16" s="74" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5403,7 +5397,7 @@
         <v>178</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>28</v>
@@ -5430,7 +5424,7 @@
         <v>28</v>
       </c>
       <c r="K18" s="74" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L18" s="74"/>
     </row>
@@ -5439,8 +5433,8 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1wcHyiuVUbBeL9ODgyYP-lyy7yM1vMH3u","5C4-017")</f>
         <v>5C4-017</v>
       </c>
-      <c r="B19" s="128" t="s">
-        <v>277</v>
+      <c r="B19" s="75" t="s">
+        <v>275</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>28</v>
@@ -5467,7 +5461,7 @@
         <v>28</v>
       </c>
       <c r="K19" s="74" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L19" s="74"/>
     </row>
@@ -5475,7 +5469,7 @@
       <c r="A20" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="150" t="s">
         <v>179</v>
       </c>
       <c r="C20" s="23" t="s">
@@ -5503,7 +5497,7 @@
         <v>175</v>
       </c>
       <c r="K20" s="74" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="L20" s="74"/>
     </row>
@@ -5540,7 +5534,7 @@
         <v>175</v>
       </c>
       <c r="K21" s="74" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L21" s="74"/>
     </row>
@@ -5577,7 +5571,7 @@
         <v>28</v>
       </c>
       <c r="K22" s="74" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L22" s="74"/>
     </row>
@@ -5607,20 +5601,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="143" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="144" t="s">
-        <v>366</v>
-      </c>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="145"/>
+      <c r="B1" s="144"/>
+      <c r="C1" s="143" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="144"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
@@ -5630,13 +5624,13 @@
         <v>163</v>
       </c>
       <c r="C2" s="68" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>366</v>
+      </c>
+      <c r="E2" s="68" t="s">
         <v>367</v>
-      </c>
-      <c r="D2" s="68" t="s">
-        <v>368</v>
-      </c>
-      <c r="E2" s="68" t="s">
-        <v>369</v>
       </c>
       <c r="F2" s="68"/>
       <c r="G2" s="69"/>
@@ -5652,10 +5646,10 @@
         <v>165</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D3" s="63" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E3" s="63"/>
       <c r="F3" s="63"/>
@@ -5666,16 +5660,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>165</v>
       </c>
       <c r="C4" s="65" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E4" s="63"/>
       <c r="F4" s="63"/>
@@ -5686,16 +5680,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B5" s="77" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D5" s="63" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
@@ -5706,7 +5700,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="55" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B6" s="57" t="s">
         <v>167</v>
@@ -5722,14 +5716,14 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B7" s="57" t="s">
         <v>168</v>
       </c>
       <c r="C7" s="65"/>
       <c r="D7" s="63" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E7" s="63"/>
       <c r="F7" s="63"/>
@@ -5746,10 +5740,10 @@
         <v>165</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E8" s="63"/>
       <c r="F8" s="63"/>
@@ -5760,16 +5754,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B9" s="56" t="s">
         <v>170</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D9" s="70" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E9" s="63"/>
       <c r="F9" s="63"/>
@@ -5780,16 +5774,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="55" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>171</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D10" s="70" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E10" s="63"/>
       <c r="F10" s="63"/>
@@ -5800,16 +5794,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B11" s="56" t="s">
         <v>172</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
@@ -5820,16 +5814,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B12" s="56" t="s">
         <v>173</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E12" s="63"/>
       <c r="F12" s="63"/>
@@ -5840,14 +5834,14 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B13" s="57" t="s">
         <v>174</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13" s="63" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E13" s="63"/>
       <c r="F13" s="63"/>
@@ -5858,14 +5852,14 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B14" s="57" t="s">
         <v>176</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="63" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E14" s="63"/>
       <c r="F14" s="63"/>
@@ -5876,16 +5870,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="55" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B15" s="56" t="s">
         <v>177</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E15" s="63"/>
       <c r="F15" s="63"/>
@@ -5902,10 +5896,10 @@
         <v>171</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D16" s="83" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E16" s="63"/>
       <c r="F16" s="63"/>
@@ -5922,10 +5916,10 @@
         <v>171</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E17" s="63"/>
       <c r="F17" s="63"/>
@@ -5942,10 +5936,10 @@
         <v>171</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E18" s="63"/>
       <c r="F18" s="63"/>
@@ -5972,7 +5966,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B20" s="57" t="s">
         <v>180</v>
@@ -5988,7 +5982,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="55" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B21" s="78" t="s">
         <v>181</v>
@@ -7406,11 +7400,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="135" t="s">
-        <v>453</v>
-      </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
+      <c r="A1" s="134" t="s">
+        <v>451</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
       <c r="D1" s="118"/>
       <c r="E1" s="118"/>
       <c r="F1" s="118"/>
@@ -7420,10 +7414,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="73" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D2" s="73"/>
       <c r="E2" s="73"/>
@@ -7435,10 +7429,10 @@
         <v>1A</v>
       </c>
       <c r="B3" s="121" t="s">
+        <v>454</v>
+      </c>
+      <c r="C3" s="123" t="s">
         <v>456</v>
-      </c>
-      <c r="C3" s="123" t="s">
-        <v>458</v>
       </c>
       <c r="D3" s="73"/>
       <c r="E3" s="73"/>
@@ -7450,7 +7444,7 @@
         <v>1B</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C4" s="123" t="s">
         <v>48</v>
@@ -7465,10 +7459,10 @@
         <v>1C</v>
       </c>
       <c r="B5" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C5" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -7480,7 +7474,7 @@
         <v>1D</v>
       </c>
       <c r="B6" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C6" s="123" t="s">
         <v>48</v>
@@ -7495,7 +7489,7 @@
         <v>1E</v>
       </c>
       <c r="B7" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C7" s="124" t="s">
         <v>48</v>
@@ -7510,10 +7504,10 @@
         <v>1F</v>
       </c>
       <c r="B8" s="121" t="s">
+        <v>454</v>
+      </c>
+      <c r="C8" s="123" t="s">
         <v>456</v>
-      </c>
-      <c r="C8" s="123" t="s">
-        <v>458</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -7525,7 +7519,7 @@
         <v>1G</v>
       </c>
       <c r="B9" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C9" s="124" t="s">
         <v>48</v>
@@ -7540,10 +7534,10 @@
         <v>1H</v>
       </c>
       <c r="B10" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C10" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -7555,7 +7549,7 @@
         <v>1J</v>
       </c>
       <c r="B11" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C11" s="123" t="s">
         <v>48</v>
@@ -7570,10 +7564,10 @@
         <v>1K</v>
       </c>
       <c r="B12" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C12" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -7585,10 +7579,10 @@
         <v>2A</v>
       </c>
       <c r="B13" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C13" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -7600,10 +7594,10 @@
         <v>2B</v>
       </c>
       <c r="B14" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C14" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -7615,7 +7609,7 @@
         <v>2C</v>
       </c>
       <c r="B15" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C15" s="123" t="s">
         <v>48</v>
@@ -7630,7 +7624,7 @@
         <v>2D</v>
       </c>
       <c r="B16" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C16" s="123" t="s">
         <v>48</v>
@@ -7645,10 +7639,10 @@
         <v>2E</v>
       </c>
       <c r="B17" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C17" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -7660,7 +7654,7 @@
         <v>2F</v>
       </c>
       <c r="B18" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C18" s="123" t="s">
         <v>48</v>
@@ -7675,7 +7669,7 @@
         <v>2G</v>
       </c>
       <c r="B19" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C19" s="123" t="s">
         <v>48</v>
@@ -7690,10 +7684,10 @@
         <v>2H</v>
       </c>
       <c r="B20" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C20" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D20" s="114"/>
       <c r="E20" s="9"/>
@@ -7705,10 +7699,10 @@
         <v>2J</v>
       </c>
       <c r="B21" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C21" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
@@ -7720,7 +7714,7 @@
         <v>2K</v>
       </c>
       <c r="B22" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C22" s="123" t="s">
         <v>48</v>
@@ -7735,7 +7729,7 @@
         <v>2L</v>
       </c>
       <c r="B23" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C23" s="123" t="s">
         <v>48</v>
@@ -7750,10 +7744,10 @@
         <v>2M</v>
       </c>
       <c r="B24" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C24" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D24" s="114"/>
       <c r="E24" s="84"/>
@@ -7765,10 +7759,10 @@
         <v>3C</v>
       </c>
       <c r="B25" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C25" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D25" s="114"/>
       <c r="E25" s="9"/>
@@ -7780,7 +7774,7 @@
         <v>3D</v>
       </c>
       <c r="B26" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C26" s="124" t="s">
         <v>48</v>
@@ -7795,7 +7789,7 @@
         <v>3E</v>
       </c>
       <c r="B27" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C27" s="123" t="s">
         <v>48</v>
@@ -7855,7 +7849,7 @@
         <v>3J</v>
       </c>
       <c r="B31" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C31" s="123" t="s">
         <v>48</v>
@@ -7870,10 +7864,10 @@
         <v>3L</v>
       </c>
       <c r="B32" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C32" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -7885,7 +7879,7 @@
         <v>4E</v>
       </c>
       <c r="B33" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C33" s="123" t="s">
         <v>48</v>
@@ -7900,7 +7894,7 @@
         <v>4F</v>
       </c>
       <c r="B34" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C34" s="123" t="s">
         <v>48</v>
@@ -7915,10 +7909,10 @@
         <v>4G</v>
       </c>
       <c r="B35" s="121" t="s">
+        <v>454</v>
+      </c>
+      <c r="C35" s="123" t="s">
         <v>456</v>
-      </c>
-      <c r="C35" s="123" t="s">
-        <v>458</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -7930,7 +7924,7 @@
         <v>4H</v>
       </c>
       <c r="B36" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C36" s="123" t="s">
         <v>48</v>
@@ -7945,10 +7939,10 @@
         <v>4J</v>
       </c>
       <c r="B37" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C37" s="123" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D37" s="114"/>
       <c r="E37" s="9"/>
@@ -7960,7 +7954,7 @@
         <v>4K</v>
       </c>
       <c r="B38" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C38" s="123" t="s">
         <v>48</v>
@@ -7975,7 +7969,7 @@
         <v>4L</v>
       </c>
       <c r="B39" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C39" s="123" t="s">
         <v>48</v>
@@ -7990,7 +7984,7 @@
         <v>5B</v>
       </c>
       <c r="B40" s="122" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C40" s="124" t="s">
         <v>48</v>
@@ -8005,10 +7999,10 @@
         <v>5C</v>
       </c>
       <c r="B41" s="121" t="s">
+        <v>454</v>
+      </c>
+      <c r="C41" s="123" t="s">
         <v>456</v>
-      </c>
-      <c r="C41" s="123" t="s">
-        <v>458</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -8020,7 +8014,7 @@
         <v>5E</v>
       </c>
       <c r="B42" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C42" s="123" t="s">
         <v>48</v>
@@ -8035,7 +8029,7 @@
         <v>5G</v>
       </c>
       <c r="B43" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C43" s="123" t="s">
         <v>48</v>
@@ -8050,7 +8044,7 @@
         <v>5H</v>
       </c>
       <c r="B44" s="121" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C44" s="123" t="s">
         <v>48</v>
@@ -8075,8 +8069,8 @@
   </sheetPr>
   <dimension ref="A1:I1023"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8088,33 +8082,33 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="92" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B1" s="93" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C1" s="93" t="s">
-        <v>426</v>
-      </c>
-      <c r="D1" s="148" t="s">
-        <v>271</v>
-      </c>
-      <c r="E1" s="148"/>
+        <v>424</v>
+      </c>
+      <c r="D1" s="147" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="147"/>
       <c r="F1" s="102" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
       <c r="G2" s="96"/>
       <c r="H2" s="96"/>
       <c r="I2" s="96"/>
     </row>
     <row r="3" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="91" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B3" s="97">
         <v>62</v>
@@ -8122,10 +8116,10 @@
       <c r="C3" s="97">
         <v>55</v>
       </c>
-      <c r="D3" s="149" t="s">
-        <v>428</v>
-      </c>
-      <c r="E3" s="150"/>
+      <c r="D3" s="148" t="s">
+        <v>426</v>
+      </c>
+      <c r="E3" s="149"/>
       <c r="F3" s="94" t="s">
         <v>261</v>
       </c>
@@ -8135,10 +8129,10 @@
     </row>
     <row r="4" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="91" t="s">
-        <v>408</v>
-      </c>
-      <c r="D4" s="150"/>
-      <c r="E4" s="150"/>
+        <v>406</v>
+      </c>
+      <c r="D4" s="149"/>
+      <c r="E4" s="149"/>
       <c r="F4" s="95"/>
       <c r="G4" s="96"/>
       <c r="H4" s="99"/>
@@ -8146,7 +8140,7 @@
     </row>
     <row r="5" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B5" s="97">
         <v>44</v>
@@ -8154,8 +8148,8 @@
       <c r="C5" s="97">
         <v>43</v>
       </c>
-      <c r="D5" s="150"/>
-      <c r="E5" s="150"/>
+      <c r="D5" s="149"/>
+      <c r="E5" s="149"/>
       <c r="F5" s="94" t="s">
         <v>261</v>
       </c>
@@ -8165,7 +8159,7 @@
     </row>
     <row r="6" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="91" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B6" s="97">
         <v>47</v>
@@ -8173,10 +8167,10 @@
       <c r="C6" s="97">
         <v>52</v>
       </c>
-      <c r="D6" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E6" s="150"/>
+      <c r="D6" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E6" s="149"/>
       <c r="F6" s="94" t="s">
         <v>261</v>
       </c>
@@ -8186,7 +8180,7 @@
     </row>
     <row r="7" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="91" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B7" s="97">
         <v>75</v>
@@ -8194,10 +8188,10 @@
       <c r="C7" s="97">
         <v>82</v>
       </c>
-      <c r="D7" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E7" s="150"/>
+      <c r="D7" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E7" s="149"/>
       <c r="F7" s="94" t="s">
         <v>261</v>
       </c>
@@ -8207,7 +8201,7 @@
     </row>
     <row r="8" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="91" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B8" s="97">
         <v>85</v>
@@ -8215,10 +8209,10 @@
       <c r="C8" s="97">
         <v>99</v>
       </c>
-      <c r="D8" s="149" t="s">
-        <v>429</v>
-      </c>
-      <c r="E8" s="150"/>
+      <c r="D8" s="148" t="s">
+        <v>427</v>
+      </c>
+      <c r="E8" s="149"/>
       <c r="F8" s="95"/>
       <c r="G8" s="96"/>
       <c r="H8" s="99"/>
@@ -8226,7 +8220,7 @@
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="91" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B9" s="97">
         <v>15</v>
@@ -8234,10 +8228,10 @@
       <c r="C9" s="97">
         <v>23</v>
       </c>
-      <c r="D9" s="149" t="s">
-        <v>428</v>
-      </c>
-      <c r="E9" s="150"/>
+      <c r="D9" s="148" t="s">
+        <v>426</v>
+      </c>
+      <c r="E9" s="149"/>
       <c r="F9" s="94" t="s">
         <v>261</v>
       </c>
@@ -8247,12 +8241,12 @@
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="91" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B10" s="98"/>
       <c r="C10" s="97"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="150"/>
+      <c r="D10" s="149"/>
+      <c r="E10" s="149"/>
       <c r="F10" s="95"/>
       <c r="G10" s="96"/>
       <c r="H10" s="99"/>
@@ -8260,12 +8254,12 @@
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="91" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B11" s="99"/>
       <c r="C11" s="97"/>
-      <c r="D11" s="150"/>
-      <c r="E11" s="150"/>
+      <c r="D11" s="149"/>
+      <c r="E11" s="149"/>
       <c r="F11" s="95"/>
       <c r="G11" s="96"/>
       <c r="H11" s="99"/>
@@ -8273,7 +8267,7 @@
     </row>
     <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="91" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B12" s="99">
         <v>57</v>
@@ -8281,10 +8275,10 @@
       <c r="C12" s="97">
         <v>59</v>
       </c>
-      <c r="D12" s="149" t="s">
-        <v>428</v>
-      </c>
-      <c r="E12" s="150"/>
+      <c r="D12" s="148" t="s">
+        <v>426</v>
+      </c>
+      <c r="E12" s="149"/>
       <c r="F12" s="94" t="s">
         <v>261</v>
       </c>
@@ -8294,7 +8288,7 @@
     </row>
     <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="91" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B13" s="99">
         <v>37</v>
@@ -8302,10 +8296,10 @@
       <c r="C13" s="97">
         <v>56</v>
       </c>
-      <c r="D13" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E13" s="150"/>
+      <c r="D13" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E13" s="149"/>
       <c r="F13" s="94" t="s">
         <v>261</v>
       </c>
@@ -8315,7 +8309,7 @@
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="91" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B14" s="99">
         <v>53</v>
@@ -8323,10 +8317,10 @@
       <c r="C14" s="97">
         <v>72</v>
       </c>
-      <c r="D14" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E14" s="150"/>
+      <c r="D14" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E14" s="149"/>
       <c r="F14" s="94" t="s">
         <v>261</v>
       </c>
@@ -8336,7 +8330,7 @@
     </row>
     <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="91" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B15" s="99">
         <v>60</v>
@@ -8344,8 +8338,8 @@
       <c r="C15" s="97">
         <v>64</v>
       </c>
-      <c r="D15" s="150"/>
-      <c r="E15" s="150"/>
+      <c r="D15" s="149"/>
+      <c r="E15" s="149"/>
       <c r="F15" s="94" t="s">
         <v>261</v>
       </c>
@@ -8355,12 +8349,12 @@
     </row>
     <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="91" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B16" s="97"/>
       <c r="C16" s="97"/>
-      <c r="D16" s="150"/>
-      <c r="E16" s="150"/>
+      <c r="D16" s="149"/>
+      <c r="E16" s="149"/>
       <c r="F16" s="95"/>
       <c r="G16" s="96"/>
       <c r="H16" s="99"/>
@@ -8368,7 +8362,7 @@
     </row>
     <row r="17" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="91" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B17" s="97">
         <v>16</v>
@@ -8376,8 +8370,8 @@
       <c r="C17" s="97">
         <v>17</v>
       </c>
-      <c r="D17" s="150"/>
-      <c r="E17" s="150"/>
+      <c r="D17" s="149"/>
+      <c r="E17" s="149"/>
       <c r="F17" s="127" t="s">
         <v>261</v>
       </c>
@@ -8387,12 +8381,12 @@
     </row>
     <row r="18" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="91" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B18" s="97"/>
       <c r="C18" s="97"/>
-      <c r="D18" s="150"/>
-      <c r="E18" s="150"/>
+      <c r="D18" s="149"/>
+      <c r="E18" s="149"/>
       <c r="F18" s="95"/>
       <c r="G18" s="96"/>
       <c r="H18" s="99"/>
@@ -8400,7 +8394,7 @@
     </row>
     <row r="19" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="91" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B19" s="97">
         <v>18</v>
@@ -8408,10 +8402,10 @@
       <c r="C19" s="97">
         <v>40</v>
       </c>
-      <c r="D19" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E19" s="150"/>
+      <c r="D19" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E19" s="149"/>
       <c r="F19" s="94" t="s">
         <v>261</v>
       </c>
@@ -8421,7 +8415,7 @@
     </row>
     <row r="20" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="91" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B20" s="97">
         <v>45</v>
@@ -8429,10 +8423,10 @@
       <c r="C20" s="97">
         <v>48</v>
       </c>
-      <c r="D20" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E20" s="150"/>
+      <c r="D20" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E20" s="149"/>
       <c r="F20" s="94" t="s">
         <v>261</v>
       </c>
@@ -8442,7 +8436,7 @@
     </row>
     <row r="21" spans="1:9" s="90" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="91" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B21" s="97">
         <v>83</v>
@@ -8450,12 +8444,12 @@
       <c r="C21" s="97">
         <v>84</v>
       </c>
-      <c r="D21" s="149" t="s">
-        <v>430</v>
-      </c>
-      <c r="E21" s="150"/>
+      <c r="D21" s="148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E21" s="149"/>
       <c r="F21" s="94" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G21" s="96"/>
       <c r="H21" s="99"/>
@@ -8566,10 +8560,10 @@
         <v>234</v>
       </c>
       <c r="B35" s="89" t="s">
+        <v>438</v>
+      </c>
+      <c r="C35" s="89" t="s">
         <v>440</v>
-      </c>
-      <c r="C35" s="89" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8577,10 +8571,10 @@
         <v>234</v>
       </c>
       <c r="B36" s="89" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C36" s="89" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8590,24 +8584,24 @@
     </row>
     <row r="38" spans="1:5" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="89" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B38" s="89" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C38" s="89" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="89" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B39" s="89" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C39" s="89" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="126" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8617,24 +8611,24 @@
     </row>
     <row r="41" spans="1:5" s="126" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="125" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B41" s="125" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C41" s="125" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="90" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="125" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B42" s="125" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C42" s="125" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D42" s="126"/>
     </row>
@@ -8646,7 +8640,7 @@
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8665,10 +8659,10 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="108" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B48" s="107" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C48" s="109"/>
       <c r="D48" s="103"/>
@@ -8676,10 +8670,10 @@
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="110" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B49" s="107" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C49" s="107"/>
       <c r="D49" s="103"/>
@@ -8694,10 +8688,10 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="108" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B51" s="107" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C51" s="109"/>
       <c r="D51" s="103"/>
@@ -8705,10 +8699,10 @@
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="110" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B52" s="107" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C52" s="107"/>
       <c r="D52" s="103"/>
@@ -8722,9 +8716,7 @@
       <c r="E53" s="103"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="108" t="s">
-        <v>415</v>
-      </c>
+      <c r="A54" s="108"/>
       <c r="B54" s="107" t="s">
         <v>262</v>
       </c>
@@ -8733,9 +8725,7 @@
       <c r="E54" s="103"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="108" t="s">
-        <v>415</v>
-      </c>
+      <c r="A55" s="108"/>
       <c r="B55" s="107" t="s">
         <v>263</v>
       </c>
@@ -8752,7 +8742,7 @@
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="105" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B57" s="104" t="s">
         <v>246</v>
@@ -8763,7 +8753,7 @@
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="105" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B58" s="104" t="s">
         <v>248</v>
@@ -8801,23 +8791,15 @@
       <c r="E62" s="103"/>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="105" t="s">
-        <v>422</v>
-      </c>
-      <c r="B63" s="104" t="s">
-        <v>264</v>
-      </c>
+      <c r="A63" s="105"/>
+      <c r="B63" s="104"/>
       <c r="C63" s="86"/>
       <c r="D63" s="103"/>
       <c r="E63" s="103"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="105" t="s">
-        <v>422</v>
-      </c>
-      <c r="B64" s="104" t="s">
-        <v>265</v>
-      </c>
+      <c r="A64" s="105"/>
+      <c r="B64" s="104"/>
       <c r="C64" s="86"/>
       <c r="D64" s="103"/>
       <c r="E64" s="103"/>
@@ -9835,7 +9817,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A3:A21 A48:B49 A51:A52 A54:A55 A57:A59" numberStoredAsText="1"/>
+    <ignoredError sqref="A3:A21 A48:B49 A51:A52 A57:A59" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9860,22 +9842,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="D1" s="47" t="s">
         <v>267</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="E1" s="47" t="s">
         <v>268</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="F1" s="47" t="s">
         <v>269</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>270</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -9883,19 +9865,19 @@
         <v>23</v>
       </c>
       <c r="B2" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="E2" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="F2" s="47" t="s">
         <v>274</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -9903,13 +9885,13 @@
         <v>97</v>
       </c>
       <c r="B3" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="48" t="s">
         <v>277</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>278</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>279</v>
       </c>
       <c r="E3" s="49"/>
       <c r="F3" s="49"/>
@@ -9919,19 +9901,19 @@
         <v>62</v>
       </c>
       <c r="B4" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" s="47" t="s">
         <v>280</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>281</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -9939,16 +9921,16 @@
         <v>142</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F5" s="50"/>
     </row>
@@ -9957,16 +9939,16 @@
         <v>58</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F6" s="50"/>
     </row>
@@ -9978,34 +9960,34 @@
         <v>179</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D7" s="47" t="s">
         <v>179</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F7" s="50"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="D8" s="47" t="s">
         <v>287</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="E8" s="47" t="s">
         <v>288</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="F8" s="47" t="s">
         <v>289</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>290</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -10013,57 +9995,57 @@
         <v>106</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F9" s="50"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="47" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B10" s="47" t="s">
         <v>181</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="47" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -10071,19 +10053,19 @@
         <v>82</v>
       </c>
       <c r="B12" s="47" t="s">
+        <v>295</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>296</v>
+      </c>
+      <c r="F12" s="47" t="s">
         <v>297</v>
-      </c>
-      <c r="C12" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>298</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -10091,16 +10073,16 @@
         <v>19</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F13" s="49"/>
     </row>
@@ -10112,16 +10094,16 @@
         <v>167</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D14" s="47" t="s">
         <v>167</v>
       </c>
       <c r="E14" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F14" s="47" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -10129,37 +10111,37 @@
         <v>85</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C15" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E15" s="47" t="s">
         <v>273</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>275</v>
       </c>
       <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B16" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C16" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D16" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E16" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -10167,53 +10149,53 @@
         <v>93</v>
       </c>
       <c r="B17" s="47" t="s">
+        <v>304</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>305</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" s="47" t="s">
         <v>306</v>
-      </c>
-      <c r="C17" s="47" t="s">
-        <v>278</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>307</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>275</v>
-      </c>
-      <c r="F17" s="47" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="47" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B18" s="47" t="s">
         <v>168</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D18" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>288</v>
+      </c>
+      <c r="F18" s="47" t="s">
         <v>289</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>290</v>
-      </c>
-      <c r="F18" s="47" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="51" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E19" s="52"/>
       <c r="F19" s="52"/>
@@ -10223,30 +10205,30 @@
         <v>140</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D20" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E20" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F20" s="47" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="47" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B21" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D21" s="47" t="s">
         <v>171</v>
@@ -10259,19 +10241,19 @@
         <v>72</v>
       </c>
       <c r="B22" s="47" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C22" s="47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D22" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>314</v>
+      </c>
+      <c r="F22" s="47" t="s">
         <v>289</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>316</v>
-      </c>
-      <c r="F22" s="47" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -10279,33 +10261,33 @@
         <v>37</v>
       </c>
       <c r="B23" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C23" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E23" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F23" s="47" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D24" s="51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E24" s="52"/>
       <c r="F24" s="52"/>
@@ -10315,39 +10297,39 @@
         <v>31</v>
       </c>
       <c r="B25" s="47" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C25" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E25" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="D25" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>275</v>
-      </c>
       <c r="F25" s="47" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="47" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B26" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E26" s="47" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F26" s="47" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -10358,13 +10340,13 @@
         <v>174</v>
       </c>
       <c r="C27" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D27" s="47" t="s">
         <v>174</v>
       </c>
       <c r="E27" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F27" s="50"/>
     </row>
@@ -10373,39 +10355,39 @@
         <v>103</v>
       </c>
       <c r="B28" s="47" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C28" s="47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D28" s="47" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E28" s="47" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F28" s="47" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="47" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C29" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D29" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E29" s="47" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F29" s="47" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -10413,39 +10395,39 @@
         <v>68</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C30" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F30" s="47" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="47" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B31" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -10453,19 +10435,19 @@
         <v>134</v>
       </c>
       <c r="B32" s="47" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C32" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -10473,17 +10455,17 @@
         <v>75</v>
       </c>
       <c r="B33" s="47" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C33" s="47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E33" s="53"/>
       <c r="F33" s="47" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -10491,16 +10473,16 @@
         <v>127</v>
       </c>
       <c r="B34" s="47" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C34" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E34" s="47" t="s">
         <v>273</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>275</v>
       </c>
       <c r="F34" s="50"/>
     </row>
@@ -10509,19 +10491,19 @@
         <v>41</v>
       </c>
       <c r="B35" s="47" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F35" s="47" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -10529,33 +10511,33 @@
         <v>100</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C36" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E36" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="D36" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E36" s="47" t="s">
-        <v>275</v>
-      </c>
       <c r="F36" s="47" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="51" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D37" s="51" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E37" s="52"/>
       <c r="F37" s="52"/>
@@ -10565,39 +10547,39 @@
         <v>115</v>
       </c>
       <c r="B38" s="47" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E38" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F38" s="47" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="47" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B39" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D39" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E39" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F39" s="47" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -10605,16 +10587,16 @@
         <v>44</v>
       </c>
       <c r="B40" s="47" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C40" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D40" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E40" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F40" s="50"/>
     </row>
@@ -10626,16 +10608,16 @@
         <v>180</v>
       </c>
       <c r="C41" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D41" s="47" t="s">
         <v>180</v>
       </c>
       <c r="E41" s="47" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F41" s="47" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -10643,19 +10625,19 @@
         <v>65</v>
       </c>
       <c r="B42" s="47" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C42" s="47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D42" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="E42" s="47" t="s">
+        <v>314</v>
+      </c>
+      <c r="F42" s="47" t="s">
         <v>289</v>
-      </c>
-      <c r="E42" s="47" t="s">
-        <v>316</v>
-      </c>
-      <c r="F42" s="47" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -10663,34 +10645,34 @@
         <v>124</v>
       </c>
       <c r="B43" s="47" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C43" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D43" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E43" s="47" t="s">
         <v>273</v>
-      </c>
-      <c r="D43" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E43" s="47" t="s">
-        <v>275</v>
       </c>
       <c r="F43" s="50"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="47" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B44" s="47" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C44" s="47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D44" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E44" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F44" s="50"/>
     </row>
@@ -10699,19 +10681,19 @@
         <v>88</v>
       </c>
       <c r="B45" s="47" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C45" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="D45" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E45" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="D45" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="E45" s="47" t="s">
-        <v>275</v>
-      </c>
       <c r="F45" s="47" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -10719,19 +10701,19 @@
         <v>130</v>
       </c>
       <c r="B46" s="47" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E46" s="47" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F46" s="47" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated feed parts inventory
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58441F2F-390A-F748-840E-E88B0ADD492B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3013534-B61F-054B-A944-3D9E25F12C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="65760" yWindow="460" windowWidth="35840" windowHeight="19760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="467">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -1446,6 +1446,9 @@
   </si>
   <si>
     <t>(010) 24 / 73</t>
+  </si>
+  <si>
+    <t>(003) 12 / 39</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1619,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1735,6 +1738,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -1965,7 +1974,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2188,6 +2197,7 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2221,16 +2231,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2474,25 +2487,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
-      <c r="O1" s="137"/>
-      <c r="P1" s="137"/>
-      <c r="Q1" s="137"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3790,38 +3803,38 @@
       <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="138" t="s">
+      <c r="A59" s="139" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="133"/>
-      <c r="C59" s="133"/>
+      <c r="B59" s="134"/>
+      <c r="C59" s="134"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="132" t="s">
+      <c r="A61" s="133" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="133"/>
-      <c r="C61" s="132" t="s">
+      <c r="B61" s="134"/>
+      <c r="C61" s="133" t="s">
         <v>158</v>
       </c>
-      <c r="D61" s="133"/>
-      <c r="E61" s="133"/>
-      <c r="F61" s="133"/>
+      <c r="D61" s="134"/>
+      <c r="E61" s="134"/>
+      <c r="F61" s="134"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="132" t="s">
+      <c r="A62" s="133" t="s">
         <v>159</v>
       </c>
-      <c r="B62" s="133"/>
-      <c r="C62" s="132" t="s">
+      <c r="B62" s="134"/>
+      <c r="C62" s="133" t="s">
         <v>160</v>
       </c>
-      <c r="D62" s="133"/>
-      <c r="E62" s="133"/>
-      <c r="F62" s="133"/>
+      <c r="D62" s="134"/>
+      <c r="E62" s="134"/>
+      <c r="F62" s="134"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4789,7 +4802,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4802,20 +4815,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="140" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="141" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
       <c r="K1" s="79"/>
       <c r="L1" s="79"/>
     </row>
@@ -4880,11 +4893,11 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1G8ecO5ODQmn8FX8jzQ962D928BpQ6iUm","5C4-002")</f>
         <v>5C4-002</v>
       </c>
-      <c r="B4" s="82" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>166</v>
+      <c r="B4" s="151" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>28</v>
@@ -4907,7 +4920,9 @@
       <c r="J4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="17"/>
+      <c r="K4" s="74" t="s">
+        <v>466</v>
+      </c>
       <c r="L4" s="17"/>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5469,8 +5484,8 @@
       <c r="A20" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="150" t="s">
-        <v>179</v>
+      <c r="B20" s="132" t="s">
+        <v>165</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>28</v>
@@ -5493,7 +5508,7 @@
       <c r="I20" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="26" t="s">
+      <c r="J20" s="152" t="s">
         <v>175</v>
       </c>
       <c r="K20" s="74" t="s">
@@ -5601,20 +5616,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="144" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="143" t="s">
+      <c r="B1" s="145"/>
+      <c r="C1" s="144" t="s">
         <v>364</v>
       </c>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="144"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="145"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="68" t="s">
@@ -7400,11 +7415,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>451</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
       <c r="D1" s="118"/>
       <c r="E1" s="118"/>
       <c r="F1" s="118"/>
@@ -8090,10 +8105,10 @@
       <c r="C1" s="93" t="s">
         <v>424</v>
       </c>
-      <c r="D1" s="147" t="s">
+      <c r="D1" s="150" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="147"/>
+      <c r="E1" s="150"/>
       <c r="F1" s="102" t="s">
         <v>434</v>
       </c>
@@ -9791,6 +9806,11 @@
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D2:E2"/>
@@ -9807,11 +9827,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Signal Processing AC Diagrams
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5260866F-82E5-AE49-B3DE-DDB961F0222F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B249F9E-9EA4-874F-8F7A-C1C5CA2063D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="470">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -2204,6 +2204,12 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2237,20 +2243,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2495,25 +2495,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
-      <c r="P1" s="143"/>
-      <c r="Q1" s="143"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="145"/>
+      <c r="K1" s="144"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3832,38 +3832,38 @@
       <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="144" t="s">
+      <c r="A59" s="146" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="139"/>
-      <c r="C59" s="139"/>
+      <c r="B59" s="141"/>
+      <c r="C59" s="141"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="138" t="s">
+      <c r="A61" s="140" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="139"/>
-      <c r="C61" s="138" t="s">
+      <c r="B61" s="141"/>
+      <c r="C61" s="140" t="s">
         <v>158</v>
       </c>
-      <c r="D61" s="139"/>
-      <c r="E61" s="139"/>
-      <c r="F61" s="139"/>
+      <c r="D61" s="141"/>
+      <c r="E61" s="141"/>
+      <c r="F61" s="141"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="138" t="s">
+      <c r="A62" s="140" t="s">
         <v>159</v>
       </c>
-      <c r="B62" s="139"/>
-      <c r="C62" s="138" t="s">
+      <c r="B62" s="141"/>
+      <c r="C62" s="140" t="s">
         <v>160</v>
       </c>
-      <c r="D62" s="139"/>
-      <c r="E62" s="139"/>
-      <c r="F62" s="139"/>
+      <c r="D62" s="141"/>
+      <c r="E62" s="141"/>
+      <c r="F62" s="141"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4844,20 +4844,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="147" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="147" t="s">
+      <c r="B1" s="148"/>
+      <c r="C1" s="149" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
       <c r="K1" s="75"/>
       <c r="L1" s="75"/>
     </row>
@@ -5675,20 +5675,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="151" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="149" t="s">
+      <c r="B1" s="152"/>
+      <c r="C1" s="151" t="s">
         <v>357</v>
       </c>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="150"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="152"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
@@ -7501,11 +7501,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="142" t="s">
         <v>438</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
       <c r="D1" s="109"/>
       <c r="E1" s="109"/>
       <c r="F1" s="109"/>
@@ -8191,18 +8191,18 @@
       <c r="C1" s="86" t="s">
         <v>415</v>
       </c>
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="157" t="s">
         <v>262</v>
       </c>
-      <c r="E1" s="153"/>
+      <c r="E1" s="157"/>
       <c r="F1" s="95" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="83" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
       <c r="G2" s="89"/>
       <c r="H2" s="89"/>
       <c r="I2" s="89"/>
@@ -8217,10 +8217,10 @@
       <c r="C3" s="90">
         <v>55</v>
       </c>
-      <c r="D3" s="154" t="s">
+      <c r="D3" s="155" t="s">
         <v>417</v>
       </c>
-      <c r="E3" s="155"/>
+      <c r="E3" s="156"/>
       <c r="F3" s="87" t="s">
         <v>254</v>
       </c>
@@ -8232,8 +8232,8 @@
       <c r="A4" s="84" t="s">
         <v>397</v>
       </c>
-      <c r="D4" s="155"/>
-      <c r="E4" s="155"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
       <c r="F4" s="88"/>
       <c r="G4" s="89"/>
       <c r="H4" s="92"/>
@@ -8249,8 +8249,8 @@
       <c r="C5" s="90">
         <v>43</v>
       </c>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
       <c r="F5" s="87" t="s">
         <v>254</v>
       </c>
@@ -8268,10 +8268,10 @@
       <c r="C6" s="90">
         <v>52</v>
       </c>
-      <c r="D6" s="154" t="s">
+      <c r="D6" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E6" s="155"/>
+      <c r="E6" s="156"/>
       <c r="F6" s="87" t="s">
         <v>254</v>
       </c>
@@ -8289,10 +8289,10 @@
       <c r="C7" s="90">
         <v>82</v>
       </c>
-      <c r="D7" s="154" t="s">
+      <c r="D7" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E7" s="155"/>
+      <c r="E7" s="156"/>
       <c r="F7" s="87" t="s">
         <v>254</v>
       </c>
@@ -8310,10 +8310,10 @@
       <c r="C8" s="90">
         <v>99</v>
       </c>
-      <c r="D8" s="154" t="s">
+      <c r="D8" s="155" t="s">
         <v>418</v>
       </c>
-      <c r="E8" s="155"/>
+      <c r="E8" s="156"/>
       <c r="F8" s="88"/>
       <c r="G8" s="89"/>
       <c r="H8" s="92"/>
@@ -8329,10 +8329,10 @@
       <c r="C9" s="90">
         <v>23</v>
       </c>
-      <c r="D9" s="154" t="s">
+      <c r="D9" s="155" t="s">
         <v>417</v>
       </c>
-      <c r="E9" s="155"/>
+      <c r="E9" s="156"/>
       <c r="F9" s="87" t="s">
         <v>254</v>
       </c>
@@ -8346,8 +8346,8 @@
       </c>
       <c r="B10" s="91"/>
       <c r="C10" s="90"/>
-      <c r="D10" s="155"/>
-      <c r="E10" s="155"/>
+      <c r="D10" s="156"/>
+      <c r="E10" s="156"/>
       <c r="F10" s="88"/>
       <c r="G10" s="89"/>
       <c r="H10" s="92"/>
@@ -8359,8 +8359,8 @@
       </c>
       <c r="B11" s="92"/>
       <c r="C11" s="90"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="155"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="156"/>
       <c r="F11" s="88"/>
       <c r="G11" s="89"/>
       <c r="H11" s="92"/>
@@ -8376,10 +8376,10 @@
       <c r="C12" s="90">
         <v>59</v>
       </c>
-      <c r="D12" s="154" t="s">
+      <c r="D12" s="155" t="s">
         <v>417</v>
       </c>
-      <c r="E12" s="155"/>
+      <c r="E12" s="156"/>
       <c r="F12" s="87" t="s">
         <v>254</v>
       </c>
@@ -8397,10 +8397,10 @@
       <c r="C13" s="90">
         <v>56</v>
       </c>
-      <c r="D13" s="154" t="s">
+      <c r="D13" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E13" s="155"/>
+      <c r="E13" s="156"/>
       <c r="F13" s="87" t="s">
         <v>254</v>
       </c>
@@ -8418,10 +8418,10 @@
       <c r="C14" s="90">
         <v>72</v>
       </c>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E14" s="155"/>
+      <c r="E14" s="156"/>
       <c r="F14" s="87" t="s">
         <v>254</v>
       </c>
@@ -8439,8 +8439,8 @@
       <c r="C15" s="90">
         <v>64</v>
       </c>
-      <c r="D15" s="155"/>
-      <c r="E15" s="155"/>
+      <c r="D15" s="156"/>
+      <c r="E15" s="156"/>
       <c r="F15" s="87" t="s">
         <v>254</v>
       </c>
@@ -8454,8 +8454,8 @@
       </c>
       <c r="B16" s="90"/>
       <c r="C16" s="90"/>
-      <c r="D16" s="155"/>
-      <c r="E16" s="155"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
       <c r="F16" s="88"/>
       <c r="G16" s="89"/>
       <c r="H16" s="92"/>
@@ -8471,8 +8471,8 @@
       <c r="C17" s="90">
         <v>17</v>
       </c>
-      <c r="D17" s="155"/>
-      <c r="E17" s="155"/>
+      <c r="D17" s="156"/>
+      <c r="E17" s="156"/>
       <c r="F17" s="118" t="s">
         <v>254</v>
       </c>
@@ -8486,8 +8486,8 @@
       </c>
       <c r="B18" s="90"/>
       <c r="C18" s="90"/>
-      <c r="D18" s="155"/>
-      <c r="E18" s="155"/>
+      <c r="D18" s="156"/>
+      <c r="E18" s="156"/>
       <c r="F18" s="88"/>
       <c r="G18" s="89"/>
       <c r="H18" s="92"/>
@@ -8503,10 +8503,10 @@
       <c r="C19" s="90">
         <v>40</v>
       </c>
-      <c r="D19" s="154" t="s">
+      <c r="D19" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E19" s="155"/>
+      <c r="E19" s="156"/>
       <c r="F19" s="87" t="s">
         <v>254</v>
       </c>
@@ -8524,10 +8524,10 @@
       <c r="C20" s="90">
         <v>48</v>
       </c>
-      <c r="D20" s="154" t="s">
+      <c r="D20" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E20" s="155"/>
+      <c r="E20" s="156"/>
       <c r="F20" s="87" t="s">
         <v>254</v>
       </c>
@@ -8545,10 +8545,10 @@
       <c r="C21" s="90">
         <v>84</v>
       </c>
-      <c r="D21" s="154" t="s">
+      <c r="D21" s="155" t="s">
         <v>419</v>
       </c>
-      <c r="E21" s="155"/>
+      <c r="E21" s="156"/>
       <c r="F21" s="87" t="s">
         <v>424</v>
       </c>
@@ -9892,6 +9892,11 @@
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D2:E2"/>
@@ -9908,11 +9913,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9931,7 +9931,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10324,20 +10324,20 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="138" t="s">
         <v>305</v>
       </c>
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="138" t="s">
         <v>278</v>
       </c>
-      <c r="C21" s="156" t="s">
+      <c r="C21" s="138" t="s">
         <v>279</v>
       </c>
-      <c r="D21" s="156" t="s">
+      <c r="D21" s="138" t="s">
         <v>298</v>
       </c>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
@@ -10632,20 +10632,22 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="156" t="s">
+      <c r="A37" s="138" t="s">
         <v>331</v>
       </c>
-      <c r="B37" s="156" t="s">
+      <c r="B37" s="138" t="s">
         <v>278</v>
       </c>
-      <c r="C37" s="156" t="s">
+      <c r="C37" s="138" t="s">
         <v>279</v>
       </c>
-      <c r="D37" s="156" t="s">
-        <v>298</v>
-      </c>
-      <c r="E37" s="157"/>
-      <c r="F37" s="157"/>
+      <c r="D37" s="138" t="s">
+        <v>280</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>272</v>
+      </c>
+      <c r="F37" s="139"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="46" t="s">

</xml_diff>

<commit_message>
added new meeting slides
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE366C2-04AE-FD47-BDBE-4DF362DF5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F35A365-E7A6-A24C-83FD-750DEFB2F25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="72780" yWindow="460" windowWidth="35840" windowHeight="19700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2203,6 +2203,9 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2236,16 +2239,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2491,25 +2491,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="142"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
-      <c r="P1" s="143"/>
-      <c r="Q1" s="143"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="144"/>
+      <c r="O1" s="144"/>
+      <c r="P1" s="144"/>
+      <c r="Q1" s="144"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3828,38 +3828,38 @@
       <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="144" t="s">
+      <c r="A59" s="145" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="139"/>
-      <c r="C59" s="139"/>
+      <c r="B59" s="140"/>
+      <c r="C59" s="140"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="138" t="s">
+      <c r="A61" s="139" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="139"/>
-      <c r="C61" s="138" t="s">
+      <c r="B61" s="140"/>
+      <c r="C61" s="139" t="s">
         <v>158</v>
       </c>
-      <c r="D61" s="139"/>
-      <c r="E61" s="139"/>
-      <c r="F61" s="139"/>
+      <c r="D61" s="140"/>
+      <c r="E61" s="140"/>
+      <c r="F61" s="140"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="138" t="s">
+      <c r="A62" s="139" t="s">
         <v>159</v>
       </c>
-      <c r="B62" s="139"/>
-      <c r="C62" s="138" t="s">
+      <c r="B62" s="140"/>
+      <c r="C62" s="139" t="s">
         <v>160</v>
       </c>
-      <c r="D62" s="139"/>
-      <c r="E62" s="139"/>
-      <c r="F62" s="139"/>
+      <c r="D62" s="140"/>
+      <c r="E62" s="140"/>
+      <c r="F62" s="140"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4827,7 +4827,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4840,20 +4840,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="147" t="s">
+      <c r="B1" s="147"/>
+      <c r="C1" s="148" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
       <c r="K1" s="75"/>
       <c r="L1" s="75"/>
     </row>
@@ -4899,8 +4899,8 @@
       <c r="A3" s="21" t="s">
         <v>437</v>
       </c>
-      <c r="B3" s="133" t="s">
-        <v>165</v>
+      <c r="B3" s="76" t="s">
+        <v>294</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>28</v>
@@ -5650,7 +5650,7 @@
         <v>470</v>
       </c>
       <c r="B23" s="130"/>
-      <c r="C23" s="156"/>
+      <c r="C23" s="138"/>
       <c r="D23" s="71"/>
       <c r="E23" s="71"/>
       <c r="F23" s="71"/>
@@ -5666,7 +5666,7 @@
         <v>471</v>
       </c>
       <c r="B24" s="130"/>
-      <c r="C24" s="156"/>
+      <c r="C24" s="138"/>
       <c r="D24" s="71"/>
       <c r="E24" s="71"/>
       <c r="F24" s="71"/>
@@ -5682,7 +5682,7 @@
         <v>472</v>
       </c>
       <c r="B25" s="130"/>
-      <c r="C25" s="156"/>
+      <c r="C25" s="138"/>
       <c r="D25" s="71"/>
       <c r="E25" s="71"/>
       <c r="F25" s="71"/>
@@ -5719,20 +5719,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
+      <c r="A1" s="150" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="149" t="s">
+      <c r="B1" s="151"/>
+      <c r="C1" s="150" t="s">
         <v>357</v>
       </c>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="150"/>
+      <c r="D1" s="152"/>
+      <c r="E1" s="152"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="152"/>
+      <c r="H1" s="152"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="151"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
@@ -7545,11 +7545,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="140" t="s">
+      <c r="A1" s="141" t="s">
         <v>438</v>
       </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
       <c r="D1" s="109"/>
       <c r="E1" s="109"/>
       <c r="F1" s="109"/>
@@ -8235,10 +8235,10 @@
       <c r="C1" s="86" t="s">
         <v>415</v>
       </c>
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="E1" s="153"/>
+      <c r="E1" s="156"/>
       <c r="F1" s="95" t="s">
         <v>421</v>
       </c>
@@ -9936,6 +9936,11 @@
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D2:E2"/>
@@ -9952,11 +9957,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update meeting slides and memo
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F35A365-E7A6-A24C-83FD-750DEFB2F25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042106DA-629E-A640-BB50-38512919C795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="72780" yWindow="460" windowWidth="35840" windowHeight="19700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1637,7 +1637,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1736,14 +1736,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1974,7 +1980,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2194,9 +2200,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2239,13 +2244,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2491,25 +2500,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
-      <c r="P1" s="144"/>
-      <c r="Q1" s="144"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="143"/>
+      <c r="N1" s="143"/>
+      <c r="O1" s="143"/>
+      <c r="P1" s="143"/>
+      <c r="Q1" s="143"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3828,38 +3837,38 @@
       <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="145" t="s">
+      <c r="A59" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="B59" s="140"/>
-      <c r="C59" s="140"/>
+      <c r="B59" s="139"/>
+      <c r="C59" s="139"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="139" t="s">
+      <c r="A61" s="138" t="s">
         <v>149</v>
       </c>
-      <c r="B61" s="140"/>
-      <c r="C61" s="139" t="s">
+      <c r="B61" s="139"/>
+      <c r="C61" s="138" t="s">
         <v>158</v>
       </c>
-      <c r="D61" s="140"/>
-      <c r="E61" s="140"/>
-      <c r="F61" s="140"/>
+      <c r="D61" s="139"/>
+      <c r="E61" s="139"/>
+      <c r="F61" s="139"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="139" t="s">
+      <c r="A62" s="138" t="s">
         <v>159</v>
       </c>
-      <c r="B62" s="140"/>
-      <c r="C62" s="139" t="s">
+      <c r="B62" s="139"/>
+      <c r="C62" s="138" t="s">
         <v>160</v>
       </c>
-      <c r="D62" s="140"/>
-      <c r="E62" s="140"/>
-      <c r="F62" s="140"/>
+      <c r="D62" s="139"/>
+      <c r="E62" s="139"/>
+      <c r="F62" s="139"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4827,7 +4836,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection sqref="A1:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4840,20 +4849,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="145" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="148" t="s">
+      <c r="B1" s="146"/>
+      <c r="C1" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="148"/>
+      <c r="I1" s="148"/>
+      <c r="J1" s="148"/>
       <c r="K1" s="75"/>
       <c r="L1" s="75"/>
     </row>
@@ -5126,7 +5135,7 @@
       <c r="A9" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="133" t="s">
+      <c r="B9" s="156" t="s">
         <v>165</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -5141,7 +5150,7 @@
       <c r="F9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="157" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="20" t="s">
@@ -5650,7 +5659,7 @@
         <v>470</v>
       </c>
       <c r="B23" s="130"/>
-      <c r="C23" s="138"/>
+      <c r="C23" s="137"/>
       <c r="D23" s="71"/>
       <c r="E23" s="71"/>
       <c r="F23" s="71"/>
@@ -5666,7 +5675,7 @@
         <v>471</v>
       </c>
       <c r="B24" s="130"/>
-      <c r="C24" s="138"/>
+      <c r="C24" s="137"/>
       <c r="D24" s="71"/>
       <c r="E24" s="71"/>
       <c r="F24" s="71"/>
@@ -5682,7 +5691,7 @@
         <v>472</v>
       </c>
       <c r="B25" s="130"/>
-      <c r="C25" s="138"/>
+      <c r="C25" s="137"/>
       <c r="D25" s="71"/>
       <c r="E25" s="71"/>
       <c r="F25" s="71"/>
@@ -5719,20 +5728,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="149" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="150" t="s">
+      <c r="B1" s="150"/>
+      <c r="C1" s="149" t="s">
         <v>357</v>
       </c>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="150"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
@@ -5912,7 +5921,7 @@
       <c r="A11" s="53" t="s">
         <v>349</v>
       </c>
-      <c r="B11" s="135" t="s">
+      <c r="B11" s="134" t="s">
         <v>165</v>
       </c>
       <c r="C11" s="60" t="s">
@@ -6028,7 +6037,7 @@
       <c r="A17" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="133" t="s">
         <v>458</v>
       </c>
       <c r="C17" s="62" t="s">
@@ -6048,7 +6057,7 @@
       <c r="A18" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="B18" s="134" t="s">
+      <c r="B18" s="133" t="s">
         <v>343</v>
       </c>
       <c r="C18" s="62" t="s">
@@ -6068,7 +6077,7 @@
       <c r="A19" s="53" t="s">
         <v>236</v>
       </c>
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="133" t="s">
         <v>268</v>
       </c>
       <c r="C19" s="62" t="s">
@@ -7545,11 +7554,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="140" t="s">
         <v>438</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
       <c r="D1" s="109"/>
       <c r="E1" s="109"/>
       <c r="F1" s="109"/>
@@ -8235,10 +8244,10 @@
       <c r="C1" s="86" t="s">
         <v>415</v>
       </c>
-      <c r="D1" s="156" t="s">
+      <c r="D1" s="153" t="s">
         <v>262</v>
       </c>
-      <c r="E1" s="156"/>
+      <c r="E1" s="153"/>
       <c r="F1" s="95" t="s">
         <v>421</v>
       </c>
@@ -9936,11 +9945,6 @@
     <row r="1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D2:E2"/>
@@ -9957,6 +9961,11 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10368,20 +10377,20 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="136" t="s">
+      <c r="A21" s="135" t="s">
         <v>305</v>
       </c>
-      <c r="B21" s="136" t="s">
+      <c r="B21" s="135" t="s">
         <v>278</v>
       </c>
-      <c r="C21" s="136" t="s">
+      <c r="C21" s="135" t="s">
         <v>279</v>
       </c>
-      <c r="D21" s="136" t="s">
+      <c r="D21" s="135" t="s">
         <v>298</v>
       </c>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
@@ -10676,22 +10685,22 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="136" t="s">
+      <c r="A37" s="135" t="s">
         <v>331</v>
       </c>
-      <c r="B37" s="136" t="s">
+      <c r="B37" s="135" t="s">
         <v>278</v>
       </c>
-      <c r="C37" s="136" t="s">
+      <c r="C37" s="135" t="s">
         <v>279</v>
       </c>
-      <c r="D37" s="136" t="s">
+      <c r="D37" s="135" t="s">
         <v>280</v>
       </c>
       <c r="E37" s="46" t="s">
         <v>272</v>
       </c>
-      <c r="F37" s="137"/>
+      <c r="F37" s="136"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="46" t="s">

</xml_diff>

<commit_message>
measured 3c and 4j
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE30830F-F510-E447-90F9-1AC453413C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FD3AEB-17CD-4141-BC1F-2DE9D7200D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20800" yWindow="460" windowWidth="14460" windowHeight="19680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="34680" windowHeight="19540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="481">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -1483,6 +1483,15 @@
   </si>
   <si>
     <t>Drive Box</t>
+  </si>
+  <si>
+    <t>3C New Cryocooler</t>
+  </si>
+  <si>
+    <t>X=0.18 Y=0.05 Z=0.18</t>
+  </si>
+  <si>
+    <t>X=0.12 Y=0.03 Z=0.09</t>
   </si>
 </sst>
 </file>
@@ -6391,10 +6400,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CEE8EE-E616-9C40-8E50-615D9D9C3993}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6831,6 +6840,26 @@
       <c r="H22" s="60"/>
       <c r="I22" s="60"/>
       <c r="J22" s="60"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>478</v>
+      </c>
+      <c r="C23" s="64" t="s">
+        <v>479</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>480</v>
+      </c>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6855,6 +6884,7 @@
     <hyperlink ref="A21" r:id="rId15" display="https://drive.google.com/drive/folders/1x-FjLa7p2gJDSbRaODzjs8ijaA9SGLtW" xr:uid="{76539FEA-D20F-504F-803D-6634EE2BA126}"/>
     <hyperlink ref="A22" r:id="rId16" display="https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr" xr:uid="{4C921AD2-E69C-7C40-B1A1-DDA3F76C36D9}"/>
     <hyperlink ref="A3" r:id="rId17" display="https://drive.google.com/drive/folders/1G8ecO5ODQmn8FX8jzQ962D928BpQ6iUm" xr:uid="{7834EE57-2441-7D43-80AF-2833C3E54227}"/>
+    <hyperlink ref="A23" r:id="rId18" display="https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr" xr:uid="{03D79150-B3F9-F74F-A7DD-3DB4FCCDA7E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8226,7 +8256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4910D-2B19-014E-928F-E015E5BABD78}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated feed parts document
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73072E81-6943-3F4D-ABF9-20031D2D76F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FA0686-B43D-7844-A46F-9A39208EE1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="81120" yWindow="460" windowWidth="34680" windowHeight="19540" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="489">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -1492,6 +1492,30 @@
   </si>
   <si>
     <t>X=0.12 Y=0.03 Z=0.09</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>QRFH</t>
+  </si>
+  <si>
+    <t>2064Z / 2287Z</t>
+  </si>
+  <si>
+    <t>5C4-024</t>
+  </si>
+  <si>
+    <t>5C4-025</t>
+  </si>
+  <si>
+    <t>5C4-026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minex </t>
+  </si>
+  <si>
+    <t>Painter</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1819,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2028,12 +2052,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2211,15 +2289,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2274,6 +2348,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2308,9 +2411,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2556,25 +2656,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="161" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="152"/>
-      <c r="I1" s="153"/>
-      <c r="J1" s="153"/>
-      <c r="K1" s="152"/>
-      <c r="L1" s="153"/>
-      <c r="M1" s="153"/>
-      <c r="N1" s="153"/>
-      <c r="O1" s="153"/>
-      <c r="P1" s="153"/>
-      <c r="Q1" s="153"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="164"/>
+      <c r="J1" s="164"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="164"/>
+      <c r="M1" s="164"/>
+      <c r="N1" s="164"/>
+      <c r="O1" s="164"/>
+      <c r="P1" s="164"/>
+      <c r="Q1" s="164"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3204,7 +3304,7 @@
       <c r="D23" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="118" t="s">
+      <c r="E23" s="117" t="s">
         <v>89</v>
       </c>
       <c r="F23" s="78"/>
@@ -3545,7 +3645,7 @@
         <f>HYPERLINK("https://drive.google.com/open?id=1nHAP6VZOPX4PWClDeQpEHh4MuzIQchEa","4G")</f>
         <v>4G</v>
       </c>
-      <c r="B35" s="145" t="s">
+      <c r="B35" s="143" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -3893,38 +3993,38 @@
       <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="154" t="s">
+      <c r="A59" s="165" t="s">
         <v>136</v>
       </c>
-      <c r="B59" s="149"/>
-      <c r="C59" s="149"/>
+      <c r="B59" s="160"/>
+      <c r="C59" s="160"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="148" t="s">
+      <c r="A61" s="159" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="149"/>
-      <c r="C61" s="148" t="s">
+      <c r="B61" s="160"/>
+      <c r="C61" s="159" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="149"/>
-      <c r="E61" s="149"/>
-      <c r="F61" s="149"/>
+      <c r="D61" s="160"/>
+      <c r="E61" s="160"/>
+      <c r="F61" s="160"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="148" t="s">
+      <c r="A62" s="159" t="s">
         <v>138</v>
       </c>
-      <c r="B62" s="149"/>
-      <c r="C62" s="148" t="s">
+      <c r="B62" s="160"/>
+      <c r="C62" s="159" t="s">
         <v>139</v>
       </c>
-      <c r="D62" s="149"/>
-      <c r="E62" s="149"/>
-      <c r="F62" s="149"/>
+      <c r="D62" s="160"/>
+      <c r="E62" s="160"/>
+      <c r="F62" s="160"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4889,10 +4989,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection sqref="A1:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4905,20 +5005,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="166" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="157" t="s">
+      <c r="B1" s="167"/>
+      <c r="C1" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="169"/>
+      <c r="H1" s="169"/>
+      <c r="I1" s="169"/>
+      <c r="J1" s="169"/>
       <c r="K1" s="75"/>
       <c r="L1" s="75"/>
     </row>
@@ -5206,7 +5306,7 @@
       <c r="F9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="116" t="s">
+      <c r="G9" s="115" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="20" t="s">
@@ -5267,10 +5367,12 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1EhIIjKRxAQ858Wo2OYQq3GdqbI2ok5Af","5C4-009")</f>
         <v>5C4-009</v>
       </c>
-      <c r="B11" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="C11" s="71"/>
+      <c r="B11" s="76" t="s">
+        <v>481</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>482</v>
+      </c>
       <c r="D11" s="20" t="s">
         <v>25</v>
       </c>
@@ -5286,9 +5388,15 @@
       <c r="H11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
+      <c r="I11" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="71" t="s">
+        <v>483</v>
+      </c>
       <c r="L11" s="71"/>
     </row>
     <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -5672,66 +5780,80 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="str">
+      <c r="A22" s="153" t="str">
         <f>HYPERLINK("https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr","5C4-020")</f>
         <v>5C4-020</v>
       </c>
-      <c r="B22" s="119" t="s">
+      <c r="B22" s="154" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="115" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="116" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K22" s="71" t="s">
+      <c r="C22" s="155" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="157" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="156" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="158" t="s">
         <v>403</v>
       </c>
-      <c r="L22" s="71" t="s">
+      <c r="L22" s="158" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="148" t="s">
         <v>404</v>
       </c>
-      <c r="B23" s="117"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
+      <c r="B23" s="149" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="150"/>
+      <c r="D23" s="151" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="151" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="151" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="157" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="157" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="152"/>
+      <c r="J23" s="152"/>
+      <c r="K23" s="152"/>
+      <c r="L23" s="152"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>405</v>
       </c>
-      <c r="B24" s="117"/>
-      <c r="C24" s="124"/>
+      <c r="B24" s="116" t="s">
+        <v>487</v>
+      </c>
+      <c r="C24" s="122"/>
       <c r="D24" s="71"/>
       <c r="E24" s="71"/>
       <c r="F24" s="71"/>
@@ -5746,8 +5868,10 @@
       <c r="A25" s="24" t="s">
         <v>406</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="124"/>
+      <c r="B25" s="116" t="s">
+        <v>487</v>
+      </c>
+      <c r="C25" s="122"/>
       <c r="D25" s="71"/>
       <c r="E25" s="71"/>
       <c r="F25" s="71"/>
@@ -5757,6 +5881,60 @@
       <c r="J25" s="71"/>
       <c r="K25" s="71"/>
       <c r="L25" s="71"/>
+    </row>
+    <row r="26" spans="1:12" s="146" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
+        <v>484</v>
+      </c>
+      <c r="B26" s="116" t="s">
+        <v>488</v>
+      </c>
+      <c r="C26" s="122"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
+    </row>
+    <row r="27" spans="1:12" s="146" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="24" t="s">
+        <v>485</v>
+      </c>
+      <c r="B27" s="116" t="s">
+        <v>488</v>
+      </c>
+      <c r="C27" s="122"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
+    </row>
+    <row r="28" spans="1:12" s="146" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="24" t="s">
+        <v>486</v>
+      </c>
+      <c r="B28" s="116" t="s">
+        <v>488</v>
+      </c>
+      <c r="C28" s="122"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5783,18 +5961,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="157" t="s">
+      <c r="A1" s="168" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="158"/>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
+      <c r="E1" s="169"/>
+      <c r="F1" s="169"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="106" t="s">
@@ -5815,16 +5993,16 @@
       <c r="F2" s="106" t="s">
         <v>436</v>
       </c>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>411</v>
       </c>
-      <c r="B3" s="126">
+      <c r="B3" s="124">
         <v>50</v>
       </c>
       <c r="C3" s="71">
@@ -5833,10 +6011,10 @@
       <c r="D3" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="126" t="s">
+      <c r="E3" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F3" s="126" t="s">
+      <c r="F3" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G3" s="85"/>
@@ -5848,7 +6026,7 @@
       <c r="A4" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="B4" s="126">
+      <c r="B4" s="124">
         <v>55</v>
       </c>
       <c r="C4" s="71">
@@ -5857,10 +6035,10 @@
       <c r="D4" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="E4" s="126" t="s">
+      <c r="E4" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F4" s="126" t="s">
+      <c r="F4" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G4" s="85"/>
@@ -5872,7 +6050,7 @@
       <c r="A5" s="21" t="s">
         <v>413</v>
       </c>
-      <c r="B5" s="126">
+      <c r="B5" s="124">
         <v>12</v>
       </c>
       <c r="C5" s="71">
@@ -5881,10 +6059,10 @@
       <c r="D5" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="E5" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F5" s="126" t="s">
+      <c r="F5" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G5" s="85"/>
@@ -5896,7 +6074,7 @@
       <c r="A6" s="21" t="s">
         <v>414</v>
       </c>
-      <c r="B6" s="126">
+      <c r="B6" s="124">
         <v>43</v>
       </c>
       <c r="C6" s="71">
@@ -5905,10 +6083,10 @@
       <c r="D6" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="126" t="s">
+      <c r="E6" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F6" s="126" t="s">
+      <c r="F6" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G6" s="85"/>
@@ -5920,7 +6098,7 @@
       <c r="A7" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="B7" s="126">
+      <c r="B7" s="124">
         <v>47</v>
       </c>
       <c r="C7" s="71">
@@ -5929,10 +6107,10 @@
       <c r="D7" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F7" s="126" t="s">
+      <c r="F7" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="85"/>
@@ -5944,7 +6122,7 @@
       <c r="A8" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="B8" s="126">
+      <c r="B8" s="124">
         <v>75</v>
       </c>
       <c r="C8" s="71">
@@ -5953,10 +6131,10 @@
       <c r="D8" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="126" t="s">
+      <c r="E8" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F8" s="126" t="s">
+      <c r="F8" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G8" s="85"/>
@@ -5968,7 +6146,7 @@
       <c r="A9" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="B9" s="126">
+      <c r="B9" s="124">
         <v>41</v>
       </c>
       <c r="C9" s="71">
@@ -5977,10 +6155,10 @@
       <c r="D9" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="126" t="s">
+      <c r="E9" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F9" s="126" t="s">
+      <c r="F9" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G9" s="85"/>
@@ -5992,7 +6170,7 @@
       <c r="A10" s="21" t="s">
         <v>418</v>
       </c>
-      <c r="B10" s="126">
+      <c r="B10" s="124">
         <v>15</v>
       </c>
       <c r="C10" s="71">
@@ -6001,10 +6179,10 @@
       <c r="D10" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="E10" s="126" t="s">
+      <c r="E10" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F10" s="126" t="s">
+      <c r="F10" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G10" s="85"/>
@@ -6013,20 +6191,20 @@
       <c r="J10" s="85"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="137" t="s">
+      <c r="A11" s="135" t="s">
         <v>419</v>
       </c>
-      <c r="B11" s="138">
+      <c r="B11" s="136">
         <v>19</v>
       </c>
-      <c r="C11" s="140">
+      <c r="C11" s="138">
         <v>21</v>
       </c>
-      <c r="D11" s="140"/>
-      <c r="E11" s="138" t="s">
+      <c r="D11" s="138"/>
+      <c r="E11" s="136" t="s">
         <v>437</v>
       </c>
-      <c r="F11" s="138"/>
+      <c r="F11" s="136"/>
       <c r="G11" s="85"/>
       <c r="H11" s="85"/>
       <c r="I11" s="85"/>
@@ -6036,7 +6214,7 @@
       <c r="A12" s="21" t="s">
         <v>420</v>
       </c>
-      <c r="B12" s="126">
+      <c r="B12" s="124">
         <v>24</v>
       </c>
       <c r="C12" s="71">
@@ -6045,10 +6223,10 @@
       <c r="D12" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="126" t="s">
+      <c r="E12" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F12" s="126" t="s">
+      <c r="F12" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G12" s="85"/>
@@ -6060,7 +6238,7 @@
       <c r="A13" s="21" t="s">
         <v>421</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="124">
         <v>57</v>
       </c>
       <c r="C13" s="71">
@@ -6069,10 +6247,10 @@
       <c r="D13" s="71" t="s">
         <v>377</v>
       </c>
-      <c r="E13" s="126" t="s">
+      <c r="E13" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F13" s="126" t="s">
+      <c r="F13" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G13" s="85"/>
@@ -6084,19 +6262,19 @@
       <c r="A14" s="21" t="s">
         <v>422</v>
       </c>
-      <c r="B14" s="126">
+      <c r="B14" s="124">
         <v>37</v>
       </c>
-      <c r="C14" s="124">
+      <c r="C14" s="122">
         <v>56</v>
       </c>
       <c r="D14" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="126" t="s">
+      <c r="E14" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F14" s="126" t="s">
+      <c r="F14" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="85"/>
@@ -6108,7 +6286,7 @@
       <c r="A15" s="21" t="s">
         <v>423</v>
       </c>
-      <c r="B15" s="126">
+      <c r="B15" s="124">
         <v>53</v>
       </c>
       <c r="C15" s="71">
@@ -6117,10 +6295,10 @@
       <c r="D15" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="126" t="s">
+      <c r="E15" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F15" s="126" t="s">
+      <c r="F15" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="85"/>
@@ -6132,7 +6310,7 @@
       <c r="A16" s="21" t="s">
         <v>424</v>
       </c>
-      <c r="B16" s="126">
+      <c r="B16" s="124">
         <v>60</v>
       </c>
       <c r="C16" s="71">
@@ -6141,10 +6319,10 @@
       <c r="D16" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="126" t="s">
+      <c r="E16" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F16" s="126" t="s">
+      <c r="F16" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G16" s="85"/>
@@ -6156,7 +6334,7 @@
       <c r="A17" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="B17" s="126">
+      <c r="B17" s="124">
         <v>45</v>
       </c>
       <c r="C17" s="71">
@@ -6165,10 +6343,10 @@
       <c r="D17" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="126" t="s">
+      <c r="E17" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F17" s="126" t="s">
+      <c r="F17" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="85"/>
@@ -6180,7 +6358,7 @@
       <c r="A18" s="21" t="s">
         <v>426</v>
       </c>
-      <c r="B18" s="126">
+      <c r="B18" s="124">
         <v>16</v>
       </c>
       <c r="C18" s="71">
@@ -6189,10 +6367,10 @@
       <c r="D18" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="126" t="s">
+      <c r="E18" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F18" s="126" t="s">
+      <c r="F18" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G18" s="85"/>
@@ -6204,7 +6382,7 @@
       <c r="A19" s="21" t="s">
         <v>427</v>
       </c>
-      <c r="B19" s="126" t="s">
+      <c r="B19" s="124" t="s">
         <v>438</v>
       </c>
       <c r="C19" s="71" t="s">
@@ -6213,10 +6391,10 @@
       <c r="D19" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="126" t="s">
+      <c r="E19" s="124" t="s">
         <v>440</v>
       </c>
-      <c r="F19" s="126" t="s">
+      <c r="F19" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G19" s="85"/>
@@ -6228,19 +6406,19 @@
       <c r="A20" s="21" t="s">
         <v>428</v>
       </c>
-      <c r="B20" s="126">
+      <c r="B20" s="124">
         <v>18</v>
       </c>
-      <c r="C20" s="124">
+      <c r="C20" s="122">
         <v>40</v>
       </c>
       <c r="D20" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="126" t="s">
+      <c r="E20" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F20" s="126" t="s">
+      <c r="F20" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G20" s="85"/>
@@ -6252,7 +6430,7 @@
       <c r="A21" s="21" t="s">
         <v>429</v>
       </c>
-      <c r="B21" s="126">
+      <c r="B21" s="124">
         <v>34</v>
       </c>
       <c r="C21" s="71">
@@ -6261,10 +6439,10 @@
       <c r="D21" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="126" t="s">
+      <c r="E21" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="124" t="s">
         <v>377</v>
       </c>
       <c r="G21" s="85"/>
@@ -6276,19 +6454,19 @@
       <c r="A22" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="B22" s="126">
+      <c r="B22" s="124">
         <v>83</v>
       </c>
-      <c r="C22" s="124">
+      <c r="C22" s="122">
         <v>84</v>
       </c>
       <c r="D22" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="126" t="s">
+      <c r="E22" s="124" t="s">
         <v>437</v>
       </c>
-      <c r="F22" s="126" t="s">
+      <c r="F22" s="124" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="85"/>
@@ -6297,96 +6475,96 @@
       <c r="J22" s="85"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="131" t="s">
+      <c r="A23" s="129" t="s">
         <v>431</v>
       </c>
-      <c r="B23" s="132" t="s">
+      <c r="B23" s="130" t="s">
         <v>452</v>
       </c>
-      <c r="C23" s="133" t="s">
+      <c r="C23" s="131" t="s">
         <v>453</v>
       </c>
-      <c r="D23" s="134"/>
-      <c r="E23" s="132" t="s">
+      <c r="D23" s="132"/>
+      <c r="E23" s="130" t="s">
         <v>440</v>
       </c>
-      <c r="F23" s="132"/>
+      <c r="F23" s="130"/>
       <c r="G23" s="85"/>
       <c r="H23" s="85"/>
       <c r="I23" s="85"/>
       <c r="J23" s="85"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="131" t="s">
+      <c r="A24" s="129" t="s">
         <v>432</v>
       </c>
-      <c r="B24" s="132" t="s">
+      <c r="B24" s="130" t="s">
         <v>454</v>
       </c>
-      <c r="C24" s="133" t="s">
+      <c r="C24" s="131" t="s">
         <v>455</v>
       </c>
-      <c r="D24" s="134"/>
-      <c r="E24" s="132" t="s">
+      <c r="D24" s="132"/>
+      <c r="E24" s="130" t="s">
         <v>440</v>
       </c>
-      <c r="F24" s="132"/>
+      <c r="F24" s="130"/>
       <c r="G24" s="85"/>
       <c r="H24" s="85"/>
       <c r="I24" s="85"/>
       <c r="J24" s="85"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="137" t="s">
+      <c r="A25" s="135" t="s">
         <v>433</v>
       </c>
-      <c r="B25" s="138" t="s">
+      <c r="B25" s="136" t="s">
         <v>460</v>
       </c>
-      <c r="C25" s="139" t="s">
+      <c r="C25" s="137" t="s">
         <v>461</v>
       </c>
-      <c r="D25" s="140"/>
-      <c r="E25" s="138" t="s">
+      <c r="D25" s="138"/>
+      <c r="E25" s="136" t="s">
         <v>440</v>
       </c>
-      <c r="F25" s="138"/>
+      <c r="F25" s="136"/>
       <c r="G25" s="85"/>
       <c r="H25" s="85"/>
       <c r="I25" s="85"/>
       <c r="J25" s="85"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="137" t="s">
+      <c r="A26" s="135" t="s">
         <v>434</v>
       </c>
-      <c r="B26" s="138">
+      <c r="B26" s="136">
         <v>30</v>
       </c>
-      <c r="C26" s="139">
+      <c r="C26" s="137">
         <v>68</v>
       </c>
-      <c r="D26" s="140"/>
-      <c r="E26" s="138" t="s">
+      <c r="D26" s="138"/>
+      <c r="E26" s="136" t="s">
         <v>437</v>
       </c>
-      <c r="F26" s="138"/>
+      <c r="F26" s="136"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="137" t="s">
+      <c r="A27" s="135" t="s">
         <v>435</v>
       </c>
-      <c r="B27" s="138">
+      <c r="B27" s="136">
         <v>3</v>
       </c>
-      <c r="C27" s="139">
+      <c r="C27" s="137">
         <v>2</v>
       </c>
-      <c r="D27" s="140"/>
-      <c r="E27" s="138" t="s">
+      <c r="D27" s="138"/>
+      <c r="E27" s="136" t="s">
         <v>437</v>
       </c>
-      <c r="F27" s="138"/>
+      <c r="F27" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6414,20 +6592,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="170" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="159" t="s">
+      <c r="B1" s="171"/>
+      <c r="C1" s="170" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="160"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="171"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
@@ -6613,7 +6791,7 @@
       <c r="A11" s="53" t="s">
         <v>318</v>
       </c>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="119" t="s">
         <v>144</v>
       </c>
       <c r="C11" s="60" t="s">
@@ -6729,7 +6907,7 @@
       <c r="A17" s="53" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="120" t="s">
+      <c r="B17" s="118" t="s">
         <v>392</v>
       </c>
       <c r="C17" s="62" t="s">
@@ -6749,7 +6927,7 @@
       <c r="A18" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="B18" s="120" t="s">
+      <c r="B18" s="118" t="s">
         <v>312</v>
       </c>
       <c r="C18" s="62" t="s">
@@ -6769,7 +6947,7 @@
       <c r="A19" s="53" t="s">
         <v>215</v>
       </c>
-      <c r="B19" s="120" t="s">
+      <c r="B19" s="118" t="s">
         <v>237</v>
       </c>
       <c r="C19" s="62" t="s">
@@ -8256,7 +8434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4910D-2B19-014E-928F-E015E5BABD78}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -8269,17 +8447,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="173" t="s">
         <v>372</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="152" t="s">
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="163" t="s">
         <v>474</v>
       </c>
-      <c r="F1" s="152"/>
-      <c r="G1" s="152"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="70" t="s">
@@ -8300,7 +8478,7 @@
       <c r="F2" s="70" t="s">
         <v>476</v>
       </c>
-      <c r="G2" s="127" t="s">
+      <c r="G2" s="125" t="s">
         <v>477</v>
       </c>
     </row>
@@ -8315,16 +8493,16 @@
       <c r="C3" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D3" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="146" t="s">
+      <c r="D3" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8339,14 +8517,14 @@
       <c r="C4" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146" t="s">
+      <c r="D4" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8361,16 +8539,16 @@
       <c r="C5" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D5" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="128" t="s">
+      <c r="D5" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="146" t="s">
+      <c r="G5" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8385,14 +8563,14 @@
       <c r="C6" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146" t="s">
+      <c r="D6" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="144"/>
+      <c r="G6" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8407,16 +8585,16 @@
       <c r="C7" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D7" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="128" t="s">
+      <c r="D7" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="146" t="s">
+      <c r="G7" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8431,16 +8609,16 @@
       <c r="C8" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D8" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="146" t="s">
+      <c r="D8" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8455,16 +8633,16 @@
       <c r="C9" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D9" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="128" t="s">
+      <c r="D9" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="146" t="s">
+      <c r="G9" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8479,16 +8657,16 @@
       <c r="C10" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D10" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="146" t="s">
+      <c r="D10" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8503,14 +8681,14 @@
       <c r="C11" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="128" t="s">
+      <c r="D11" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="103"/>
-      <c r="G11" s="146" t="s">
+      <c r="G11" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8525,16 +8703,16 @@
       <c r="C12" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D12" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="146" t="s">
+      <c r="D12" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8549,16 +8727,16 @@
       <c r="C13" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="146" t="s">
+      <c r="D13" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8573,16 +8751,16 @@
       <c r="C14" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D14" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="146" t="s">
+      <c r="D14" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8597,16 +8775,16 @@
       <c r="C15" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D15" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="146" t="s">
+      <c r="D15" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8621,14 +8799,14 @@
       <c r="C16" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="146"/>
-      <c r="G16" s="146" t="s">
+      <c r="D16" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8643,16 +8821,16 @@
       <c r="C17" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D17" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="146" t="s">
+      <c r="D17" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8667,14 +8845,14 @@
       <c r="C18" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="146"/>
-      <c r="G18" s="146" t="s">
+      <c r="D18" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="144"/>
+      <c r="G18" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8689,14 +8867,14 @@
       <c r="C19" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="128" t="s">
+      <c r="D19" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="103"/>
-      <c r="G19" s="146" t="s">
+      <c r="G19" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8711,16 +8889,16 @@
       <c r="C20" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="146" t="s">
+      <c r="D20" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8735,16 +8913,16 @@
       <c r="C21" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="146" t="s">
+      <c r="D21" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8759,16 +8937,16 @@
       <c r="C22" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="164" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="146" t="s">
+      <c r="D22" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="147" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8783,16 +8961,16 @@
       <c r="C23" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D23" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="146" t="s">
+      <c r="D23" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8807,16 +8985,16 @@
       <c r="C24" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D24" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="128" t="s">
+      <c r="D24" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F24" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="146" t="s">
+      <c r="G24" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8831,16 +9009,16 @@
       <c r="C25" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D25" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="146" t="s">
+      <c r="D25" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8855,16 +9033,16 @@
       <c r="C26" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D26" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="128" t="s">
+      <c r="D26" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="146" t="s">
+      <c r="G26" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8879,14 +9057,14 @@
       <c r="C27" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="146"/>
-      <c r="G27" s="146" t="s">
+      <c r="D27" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="144"/>
+      <c r="G27" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8901,10 +9079,10 @@
       <c r="C28" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="128"/>
-      <c r="E28" s="128"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126"/>
       <c r="F28" s="103"/>
-      <c r="G28" s="146"/>
+      <c r="G28" s="144"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="99" t="str">
@@ -8917,10 +9095,10 @@
       <c r="C29" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
       <c r="F29" s="103"/>
-      <c r="G29" s="146"/>
+      <c r="G29" s="144"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="99" t="str">
@@ -8933,10 +9111,10 @@
       <c r="C30" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="128"/>
-      <c r="E30" s="128"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="126"/>
       <c r="F30" s="103"/>
-      <c r="G30" s="146"/>
+      <c r="G30" s="144"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="99" t="str">
@@ -8949,14 +9127,14 @@
       <c r="C31" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="146"/>
-      <c r="G31" s="146" t="s">
+      <c r="D31" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="144"/>
+      <c r="G31" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8971,16 +9149,16 @@
       <c r="C32" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D32" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="146" t="s">
+      <c r="D32" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8995,16 +9173,16 @@
       <c r="C33" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D33" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="128" t="s">
+      <c r="D33" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F33" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="146" t="s">
+      <c r="G33" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9019,14 +9197,14 @@
       <c r="C34" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="128" t="s">
+      <c r="D34" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="103"/>
-      <c r="G34" s="146" t="s">
+      <c r="G34" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9041,16 +9219,16 @@
       <c r="C35" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D35" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="147" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="146" t="s">
+      <c r="D35" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="145" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9065,14 +9243,14 @@
       <c r="C36" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="128" t="s">
+      <c r="D36" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="126" t="s">
         <v>25</v>
       </c>
       <c r="F36" s="103"/>
-      <c r="G36" s="146" t="s">
+      <c r="G36" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9087,16 +9265,16 @@
       <c r="C37" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D37" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="146" t="s">
+      <c r="D37" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9111,14 +9289,14 @@
       <c r="C38" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="146"/>
-      <c r="G38" s="146" t="s">
+      <c r="D38" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="144"/>
+      <c r="G38" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9133,14 +9311,14 @@
       <c r="C39" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="146"/>
-      <c r="G39" s="146" t="s">
+      <c r="D39" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="144"/>
+      <c r="G39" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9155,16 +9333,16 @@
       <c r="C40" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D40" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="146" t="s">
+      <c r="D40" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9179,16 +9357,16 @@
       <c r="C41" s="103" t="s">
         <v>377</v>
       </c>
-      <c r="D41" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="146" t="s">
+      <c r="D41" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="144" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9203,14 +9381,14 @@
       <c r="C42" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="146"/>
-      <c r="G42" s="146" t="s">
+      <c r="D42" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="144"/>
+      <c r="G42" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9225,14 +9403,14 @@
       <c r="C43" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="146"/>
-      <c r="G43" s="146" t="s">
+      <c r="D43" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="144"/>
+      <c r="G43" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9247,14 +9425,14 @@
       <c r="C44" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="128" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="146"/>
-      <c r="G44" s="146" t="s">
+      <c r="D44" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="144"/>
+      <c r="G44" s="144" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9295,30 +9473,30 @@
       <c r="I1" s="84"/>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="141" t="s">
+      <c r="A3" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="139" t="s">
         <v>456</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="139" t="s">
         <v>457</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
-    </row>
-    <row r="4" spans="1:9" s="130" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="141" t="s">
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+    </row>
+    <row r="4" spans="1:9" s="128" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="139" t="s">
         <v>225</v>
       </c>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -9326,73 +9504,73 @@
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="135" t="s">
+      <c r="A6" s="133" t="s">
         <v>434</v>
       </c>
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="133" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136" t="s">
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="135" t="s">
+      <c r="A7" s="133" t="s">
         <v>434</v>
       </c>
-      <c r="B7" s="135" t="s">
+      <c r="B7" s="133" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136" t="s">
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="135" t="s">
+      <c r="A8" s="133" t="s">
         <v>419</v>
       </c>
-      <c r="B8" s="135" t="s">
+      <c r="B8" s="133" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="135" t="s">
+      <c r="C8" s="133" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136" t="s">
+      <c r="D8" s="134"/>
+      <c r="E8" s="134" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="135" t="s">
+      <c r="A9" s="133" t="s">
         <v>419</v>
       </c>
-      <c r="B9" s="135" t="s">
+      <c r="B9" s="133" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="135" t="s">
+      <c r="C9" s="133" t="s">
         <v>221</v>
       </c>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136" t="s">
+      <c r="D9" s="134"/>
+      <c r="E9" s="134" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="135" t="s">
+      <c r="A11" s="133" t="s">
         <v>144</v>
       </c>
-      <c r="B11" s="135" t="s">
+      <c r="B11" s="133" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="135" t="s">
+      <c r="C11" s="133" t="s">
         <v>463</v>
       </c>
-      <c r="D11" s="136"/>
-      <c r="E11" s="135" t="s">
+      <c r="D11" s="134"/>
+      <c r="E11" s="133" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9403,17 +9581,17 @@
       <c r="C13" s="82"/>
     </row>
     <row r="14" spans="1:9" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="141" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="141" t="s">
         <v>366</v>
       </c>
-      <c r="C14" s="143" t="s">
+      <c r="C14" s="141" t="s">
         <v>368</v>
       </c>
-      <c r="D14" s="144"/>
-      <c r="E14" s="144"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
     </row>
     <row r="15" spans="1:9" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
@@ -9425,7 +9603,7 @@
       <c r="C15" s="82" t="s">
         <v>368</v>
       </c>
-      <c r="E15" s="129"/>
+      <c r="E15" s="127"/>
     </row>
     <row r="16" spans="1:9" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="82"/>
@@ -9433,32 +9611,32 @@
       <c r="C16" s="82"/>
     </row>
     <row r="17" spans="1:5" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="135" t="s">
+      <c r="A17" s="133" t="s">
         <v>433</v>
       </c>
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="133" t="s">
         <v>380</v>
       </c>
-      <c r="C17" s="135" t="s">
+      <c r="C17" s="133" t="s">
         <v>459</v>
       </c>
-      <c r="D17" s="136"/>
-      <c r="E17" s="135" t="s">
+      <c r="D17" s="134"/>
+      <c r="E17" s="133" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="133" t="s">
         <v>433</v>
       </c>
-      <c r="B18" s="135" t="s">
+      <c r="B18" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="C18" s="135" t="s">
+      <c r="C18" s="133" t="s">
         <v>459</v>
       </c>
-      <c r="D18" s="136"/>
-      <c r="E18" s="135" t="s">
+      <c r="D18" s="134"/>
+      <c r="E18" s="133" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9468,32 +9646,32 @@
       <c r="C19" s="104"/>
     </row>
     <row r="20" spans="1:5" s="105" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="135" t="s">
+      <c r="A20" s="133" t="s">
         <v>435</v>
       </c>
-      <c r="B20" s="135" t="s">
+      <c r="B20" s="133" t="s">
         <v>369</v>
       </c>
-      <c r="C20" s="135" t="s">
+      <c r="C20" s="133" t="s">
         <v>458</v>
       </c>
-      <c r="D20" s="136"/>
-      <c r="E20" s="135" t="s">
+      <c r="D20" s="134"/>
+      <c r="E20" s="133" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="83" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="133" t="s">
         <v>435</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="133" t="s">
         <v>381</v>
       </c>
-      <c r="C21" s="135" t="s">
+      <c r="C21" s="133" t="s">
         <v>458</v>
       </c>
-      <c r="D21" s="136"/>
-      <c r="E21" s="135" t="s">
+      <c r="D21" s="134"/>
+      <c r="E21" s="133" t="s">
         <v>217</v>
       </c>
     </row>
@@ -11035,20 +11213,20 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="122" t="s">
+      <c r="A21" s="120" t="s">
         <v>274</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="120" t="s">
         <v>247</v>
       </c>
-      <c r="C21" s="122" t="s">
+      <c r="C21" s="120" t="s">
         <v>248</v>
       </c>
-      <c r="D21" s="122" t="s">
+      <c r="D21" s="120" t="s">
         <v>267</v>
       </c>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="121"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="46" t="s">
@@ -11343,22 +11521,22 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="122" t="s">
+      <c r="A37" s="120" t="s">
         <v>300</v>
       </c>
-      <c r="B37" s="122" t="s">
+      <c r="B37" s="120" t="s">
         <v>247</v>
       </c>
-      <c r="C37" s="122" t="s">
+      <c r="C37" s="120" t="s">
         <v>248</v>
       </c>
-      <c r="D37" s="122" t="s">
+      <c r="D37" s="120" t="s">
         <v>249</v>
       </c>
       <c r="E37" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="F37" s="123"/>
+      <c r="F37" s="121"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="46" t="s">

</xml_diff>

<commit_message>
added 48V check column
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA1E08A-2AC1-704A-A0FB-9E92791DA29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5511DC-DFCF-484A-9322-9D7DB78CD6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="69720" yWindow="3820" windowWidth="35840" windowHeight="20280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="437">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -6853,7 +6853,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6955,7 +6955,9 @@
       <c r="G4" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="83"/>
+      <c r="H4" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="96" t="str">
@@ -7138,7 +7140,9 @@
       <c r="G11" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="83"/>
+      <c r="H11" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="95" t="str">
@@ -7269,7 +7273,9 @@
       <c r="G16" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="83"/>
+      <c r="H16" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="95" t="str">
@@ -7344,7 +7350,9 @@
       <c r="G19" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="83"/>
+      <c r="H19" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="95" t="str">
@@ -7556,7 +7564,9 @@
       <c r="G27" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="83"/>
+      <c r="H27" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="95" t="str">
@@ -7590,7 +7600,9 @@
       <c r="E29" s="58"/>
       <c r="F29" s="58"/>
       <c r="G29" s="83"/>
-      <c r="H29" s="83"/>
+      <c r="H29" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="95" t="str">
@@ -7607,7 +7619,9 @@
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
+      <c r="H30" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="95" t="str">
@@ -7630,7 +7644,9 @@
       <c r="G31" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="83"/>
+      <c r="H31" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="95" t="str">
@@ -7707,7 +7723,9 @@
       <c r="G34" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H34" s="83"/>
+      <c r="H34" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="95" t="str">
@@ -7757,7 +7775,9 @@
       <c r="G36" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="83"/>
+      <c r="H36" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="95" t="str">
@@ -7807,7 +7827,9 @@
       <c r="G38" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H38" s="83"/>
+      <c r="H38" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="95" t="str">
@@ -7830,7 +7852,9 @@
       <c r="G39" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H39" s="83"/>
+      <c r="H39" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="95" t="str">
@@ -7907,7 +7931,9 @@
       <c r="G42" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H42" s="83"/>
+      <c r="H42" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="95" t="str">
@@ -7930,7 +7956,9 @@
       <c r="G43" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H43" s="83"/>
+      <c r="H43" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="95" t="str">
@@ -7953,7 +7981,9 @@
       <c r="G44" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="H44" s="83"/>
+      <c r="H44" s="84" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added tsys measurement for 2a
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BC96A6-C0CA-C14D-8645-48292D58D286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA928F-59FF-8E48-9BD9-D600CCEDA729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-76500" yWindow="500" windowWidth="34200" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="xx_1" localSheetId="0">'Parts At ATA'!$A$2:$G$44</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="425">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -987,12 +987,6 @@
     <t>X=0.22 Y=0.08 Z=0.18</t>
   </si>
   <si>
-    <t>X=0.12 Y=0.07 Z=0.22</t>
-  </si>
-  <si>
-    <t>X=0.11 Y=0.03 Z=0.09</t>
-  </si>
-  <si>
     <t>(019) 34 / 46</t>
   </si>
   <si>
@@ -1254,9 +1248,6 @@
     <t>Drive Box</t>
   </si>
   <si>
-    <t>3C New Cryocooler</t>
-  </si>
-  <si>
     <t>X=0.18 Y=0.05 Z=0.18</t>
   </si>
   <si>
@@ -1318,6 +1309,15 @@
   </si>
   <si>
     <t>PY Number</t>
+  </si>
+  <si>
+    <t>X=0.21 Y=0.10 Z=0.13</t>
+  </si>
+  <si>
+    <t>X=0.07 Y=0.03 Z=0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3C </t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1325,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="000"/>
+    <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -2035,6 +2035,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2074,24 +2092,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2335,25 +2335,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="108"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2394,7 +2394,7 @@
         <v>1A</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
@@ -2431,7 +2431,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>225</v>
@@ -2486,13 +2486,13 @@
         <v>1D</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>180</v>
@@ -2515,7 +2515,7 @@
         <v>1E</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>29</v>
@@ -2576,7 +2576,7 @@
         <v>1G</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>35</v>
@@ -2694,7 +2694,7 @@
         <v>2A</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>47</v>
@@ -2757,7 +2757,7 @@
         <v>2C</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>54</v>
@@ -2786,13 +2786,13 @@
         <v>2D</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>21</v>
@@ -2852,7 +2852,7 @@
         <v>62</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>106</v>
@@ -2932,7 +2932,7 @@
         <v>2J</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>71</v>
@@ -3019,7 +3019,7 @@
         <v>2M</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>80</v>
@@ -3049,7 +3049,7 @@
         <v>3C</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>81</v>
@@ -3231,7 +3231,7 @@
         <v>3J</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>88</v>
@@ -3256,7 +3256,7 @@
         <v>3L</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>90</v>
@@ -3343,7 +3343,7 @@
         <v>4G</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>97</v>
@@ -3431,7 +3431,7 @@
         <v>4K</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>105</v>
@@ -3456,7 +3456,7 @@
         <v>4L</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>107</v>
@@ -3481,7 +3481,7 @@
         <v>5B</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>109</v>
@@ -3541,13 +3541,13 @@
         <v>5E</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>117</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>85</v>
@@ -3570,7 +3570,7 @@
         <v>5G</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>118</v>
@@ -3665,28 +3665,28 @@
       <c r="A58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="102"/>
-      <c r="B59" s="97"/>
-      <c r="C59" s="97"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="105"/>
+      <c r="C59" s="105"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="96"/>
-      <c r="B61" s="97"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
-      <c r="F61" s="97"/>
+      <c r="A61" s="104"/>
+      <c r="B61" s="105"/>
+      <c r="C61" s="104"/>
+      <c r="D61" s="105"/>
+      <c r="E61" s="105"/>
+      <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="96"/>
-      <c r="B62" s="97"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="97"/>
-      <c r="E62" s="97"/>
-      <c r="F62" s="97"/>
+      <c r="A62" s="104"/>
+      <c r="B62" s="105"/>
+      <c r="C62" s="104"/>
+      <c r="D62" s="105"/>
+      <c r="E62" s="105"/>
+      <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4653,7 +4653,7 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -4668,20 +4668,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="111" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="105" t="s">
+      <c r="B1" s="112"/>
+      <c r="C1" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
@@ -4723,7 +4723,7 @@
         <v>281</v>
       </c>
       <c r="M2" s="56" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -4758,10 +4758,10 @@
         <v>25</v>
       </c>
       <c r="K3" s="38" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L3" s="38"/>
-      <c r="M3" s="116"/>
+      <c r="M3" s="99"/>
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="str">
@@ -4799,7 +4799,7 @@
         <v>311</v>
       </c>
       <c r="L4" s="12"/>
-      <c r="M4" s="116"/>
+      <c r="M4" s="99"/>
     </row>
     <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="str">
@@ -4834,10 +4834,10 @@
         <v>25</v>
       </c>
       <c r="K5" s="38" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L5" s="38"/>
-      <c r="M5" s="116"/>
+      <c r="M5" s="99"/>
     </row>
     <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="str">
@@ -4877,7 +4877,7 @@
       <c r="L6" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="M6" s="116"/>
+      <c r="M6" s="99"/>
     </row>
     <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="str">
@@ -4912,12 +4912,12 @@
         <v>131</v>
       </c>
       <c r="K7" s="43" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L7" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="M7" s="116"/>
+        <v>320</v>
+      </c>
+      <c r="M7" s="99"/>
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="str">
@@ -4952,12 +4952,12 @@
         <v>25</v>
       </c>
       <c r="K8" s="38" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L8" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="M8" s="116"/>
+        <v>320</v>
+      </c>
+      <c r="M8" s="99"/>
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
@@ -4994,7 +4994,7 @@
         <v>290</v>
       </c>
       <c r="L9" s="38"/>
-      <c r="M9" s="116"/>
+      <c r="M9" s="99"/>
     </row>
     <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="str">
@@ -5034,7 +5034,7 @@
       <c r="L10" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="M10" s="116"/>
+      <c r="M10" s="99"/>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="str">
@@ -5042,10 +5042,10 @@
         <v>5C4-009</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>25</v>
@@ -5069,10 +5069,10 @@
         <v>131</v>
       </c>
       <c r="K11" s="38" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="L11" s="38"/>
-      <c r="M11" s="116"/>
+      <c r="M11" s="99"/>
     </row>
     <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="str">
@@ -5110,7 +5110,7 @@
         <v>310</v>
       </c>
       <c r="L12" s="38"/>
-      <c r="M12" s="116"/>
+      <c r="M12" s="99"/>
     </row>
     <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="str">
@@ -5150,7 +5150,7 @@
       <c r="L13" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="M13" s="116"/>
+      <c r="M13" s="99"/>
     </row>
     <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="str">
@@ -5185,12 +5185,12 @@
         <v>131</v>
       </c>
       <c r="K14" s="43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L14" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="M14" s="116"/>
+        <v>320</v>
+      </c>
+      <c r="M14" s="99"/>
     </row>
     <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="str">
@@ -5225,12 +5225,12 @@
         <v>25</v>
       </c>
       <c r="K15" s="38" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L15" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="M15" s="116"/>
+        <v>320</v>
+      </c>
+      <c r="M15" s="99"/>
     </row>
     <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="str">
@@ -5270,7 +5270,7 @@
       <c r="L16" s="38" t="s">
         <v>283</v>
       </c>
-      <c r="M16" s="116"/>
+      <c r="M16" s="99"/>
     </row>
     <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="str">
@@ -5278,7 +5278,7 @@
         <v>5C4-015</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>25</v>
@@ -5305,16 +5305,16 @@
         <v>25</v>
       </c>
       <c r="K17" s="38" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L17" s="38"/>
-      <c r="M17" s="116"/>
+      <c r="M17" s="99"/>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="120" t="s">
+      <c r="B18" s="103" t="s">
         <v>237</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -5345,7 +5345,7 @@
         <v>304</v>
       </c>
       <c r="L18" s="38"/>
-      <c r="M18" s="116"/>
+      <c r="M18" s="99"/>
     </row>
     <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="str">
@@ -5383,7 +5383,7 @@
         <v>309</v>
       </c>
       <c r="L19" s="38"/>
-      <c r="M19" s="116"/>
+      <c r="M19" s="99"/>
     </row>
     <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
@@ -5417,12 +5417,12 @@
         <v>25</v>
       </c>
       <c r="K20" s="38" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L20" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="M20" s="116"/>
+        <v>320</v>
+      </c>
+      <c r="M20" s="99"/>
     </row>
     <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="str">
@@ -5457,19 +5457,19 @@
         <v>131</v>
       </c>
       <c r="K21" s="38" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L21" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="M21" s="116"/>
+        <v>320</v>
+      </c>
+      <c r="M21" s="99"/>
     </row>
     <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="77" t="str">
         <f>HYPERLINK("https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr","5C4-020")</f>
         <v>5C4-020</v>
       </c>
-      <c r="B22" s="119" t="s">
+      <c r="B22" s="102" t="s">
         <v>135</v>
       </c>
       <c r="C22" s="78" t="s">
@@ -5497,18 +5497,18 @@
         <v>25</v>
       </c>
       <c r="K22" s="81" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L22" s="81" t="s">
-        <v>322</v>
-      </c>
-      <c r="M22" s="117">
+        <v>320</v>
+      </c>
+      <c r="M22" s="100">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="75" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B23" s="87" t="s">
         <v>191</v>
@@ -5538,16 +5538,16 @@
         <v>25</v>
       </c>
       <c r="K23" s="81" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="L23" s="12"/>
-      <c r="M23" s="118">
+      <c r="M23" s="101">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B24" s="87" t="s">
         <v>205</v>
@@ -5577,16 +5577,16 @@
         <v>25</v>
       </c>
       <c r="K24" s="81" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="L24" s="38"/>
-      <c r="M24" s="118">
+      <c r="M24" s="101">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B25" s="87" t="s">
         <v>200</v>
@@ -5616,16 +5616,16 @@
         <v>25</v>
       </c>
       <c r="K25" s="81" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L25" s="38"/>
-      <c r="M25" s="118">
+      <c r="M25" s="101">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B26" s="87" t="s">
         <v>157</v>
@@ -5655,16 +5655,16 @@
         <v>25</v>
       </c>
       <c r="K26" s="38" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="L26" s="38"/>
-      <c r="M26" s="118">
+      <c r="M26" s="101">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B27" s="87" t="s">
         <v>232</v>
@@ -5694,19 +5694,19 @@
         <v>25</v>
       </c>
       <c r="K27" s="38" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="L27" s="38"/>
-      <c r="M27" s="118">
+      <c r="M27" s="101">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C28" s="61"/>
       <c r="D28" s="76" t="s">
@@ -5726,7 +5726,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="38"/>
       <c r="L28" s="38"/>
-      <c r="M28" s="116"/>
+      <c r="M28" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5753,14 +5753,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
-        <v>332</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="A1" s="113" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
       <c r="G1" s="62"/>
       <c r="H1" s="62"/>
       <c r="I1" s="62"/>
@@ -5771,19 +5771,19 @@
         <v>123</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>281</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B3" s="63">
         <v>50</v>
@@ -5804,7 +5804,7 @@
         <v>42</v>
       </c>
       <c r="E3" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F3" s="63" t="s">
         <v>302</v>
@@ -5816,7 +5816,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B4" s="63">
         <v>55</v>
@@ -5828,7 +5828,7 @@
         <v>302</v>
       </c>
       <c r="E4" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F4" s="63" t="s">
         <v>302</v>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B5" s="63">
         <v>12</v>
@@ -5852,7 +5852,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F5" s="63" t="s">
         <v>302</v>
@@ -5864,7 +5864,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B6" s="63">
         <v>43</v>
@@ -5876,7 +5876,7 @@
         <v>42</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F6" s="63" t="s">
         <v>302</v>
@@ -5888,7 +5888,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B7" s="63">
         <v>47</v>
@@ -5900,7 +5900,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F7" s="63" t="s">
         <v>42</v>
@@ -5912,7 +5912,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B8" s="63">
         <v>75</v>
@@ -5924,7 +5924,7 @@
         <v>42</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F8" s="63" t="s">
         <v>42</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B9" s="63">
         <v>41</v>
@@ -5948,7 +5948,7 @@
         <v>42</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F9" s="63" t="s">
         <v>302</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B10" s="63">
         <v>15</v>
@@ -5972,7 +5972,7 @@
         <v>302</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F10" s="63" t="s">
         <v>302</v>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="66" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B11" s="67">
         <v>19</v>
@@ -5994,7 +5994,7 @@
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="67" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F11" s="67" t="s">
         <v>302</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B12" s="63">
         <v>24</v>
@@ -6018,7 +6018,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F12" s="63" t="s">
         <v>302</v>
@@ -6030,7 +6030,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B13" s="63">
         <v>57</v>
@@ -6042,7 +6042,7 @@
         <v>302</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F13" s="63" t="s">
         <v>302</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B14" s="63">
         <v>37</v>
@@ -6066,7 +6066,7 @@
         <v>42</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F14" s="63" t="s">
         <v>42</v>
@@ -6078,7 +6078,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B15" s="63">
         <v>53</v>
@@ -6090,7 +6090,7 @@
         <v>42</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F15" s="63" t="s">
         <v>42</v>
@@ -6102,7 +6102,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B16" s="63">
         <v>60</v>
@@ -6114,7 +6114,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F16" s="63" t="s">
         <v>302</v>
@@ -6126,7 +6126,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B17" s="63">
         <v>45</v>
@@ -6138,7 +6138,7 @@
         <v>42</v>
       </c>
       <c r="E17" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F17" s="63" t="s">
         <v>42</v>
@@ -6149,22 +6149,22 @@
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="113" t="s">
-        <v>351</v>
-      </c>
-      <c r="B18" s="114">
+      <c r="A18" s="96" t="s">
+        <v>349</v>
+      </c>
+      <c r="B18" s="97">
         <v>16</v>
       </c>
-      <c r="C18" s="115">
+      <c r="C18" s="98">
         <v>17</v>
       </c>
-      <c r="D18" s="115" t="s">
+      <c r="D18" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="114" t="s">
-        <v>362</v>
-      </c>
-      <c r="F18" s="114" t="s">
+      <c r="E18" s="97" t="s">
+        <v>360</v>
+      </c>
+      <c r="F18" s="97" t="s">
         <v>302</v>
       </c>
       <c r="G18" s="4"/>
@@ -6174,19 +6174,19 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="63" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F19" s="63" t="s">
         <v>302</v>
@@ -6198,7 +6198,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B20" s="63">
         <v>18</v>
@@ -6210,7 +6210,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F20" s="63" t="s">
         <v>42</v>
@@ -6222,7 +6222,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B21" s="63">
         <v>34</v>
@@ -6234,7 +6234,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F21" s="63" t="s">
         <v>302</v>
@@ -6246,7 +6246,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="95" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B22" s="63">
         <v>83</v>
@@ -6258,7 +6258,7 @@
         <v>42</v>
       </c>
       <c r="E22" s="63" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F22" s="63" t="s">
         <v>302</v>
@@ -6270,19 +6270,19 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="88" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B23" s="89" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C23" s="90" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D23" s="91" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="89" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F23" s="89" t="s">
         <v>302</v>
@@ -6294,19 +6294,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="88" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B24" s="89" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D24" s="91" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="89" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F24" s="89" t="s">
         <v>302</v>
@@ -6318,19 +6318,19 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="88" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B25" s="89" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C25" s="90" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D25" s="91" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="89" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F25" s="89" t="s">
         <v>302</v>
@@ -6342,7 +6342,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="88" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B26" s="89">
         <v>30</v>
@@ -6354,7 +6354,7 @@
         <v>42</v>
       </c>
       <c r="E26" s="89" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F26" s="89" t="s">
         <v>302</v>
@@ -6362,7 +6362,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="88" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B27" s="89">
         <v>3</v>
@@ -6374,7 +6374,7 @@
         <v>42</v>
       </c>
       <c r="E27" s="89" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F27" s="89" t="s">
         <v>302</v>
@@ -6392,10 +6392,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CEE8EE-E616-9C40-8E50-615D9D9C3993}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6406,20 +6406,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="115" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="107" t="s">
+      <c r="B1" s="116"/>
+      <c r="C1" s="115" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="108"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="116"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
@@ -6438,7 +6438,7 @@
         <v>254</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G2" s="37"/>
       <c r="H2" s="30"/>
@@ -6454,7 +6454,7 @@
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="32" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
@@ -6571,10 +6571,10 @@
         <v>264</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
@@ -6606,7 +6606,7 @@
         <v>243</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>261</v>
@@ -6722,7 +6722,7 @@
         <v>139</v>
       </c>
       <c r="B17" s="60" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>265</v>
@@ -6818,13 +6818,13 @@
         <v>250</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>135</v>
+        <v>424</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>314</v>
+        <v>401</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>315</v>
+        <v>402</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
@@ -6834,18 +6834,14 @@
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>403</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>404</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>405</v>
-      </c>
+      <c r="A23" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="C23" s="36"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
@@ -6855,13 +6851,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>191</v>
+        <v>328</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>205</v>
       </c>
       <c r="C24" s="36"/>
-      <c r="D24" s="32"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="32"/>
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
@@ -6871,10 +6867,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
@@ -6887,13 +6883,15 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
-        <v>331</v>
+        <v>405</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
+      <c r="D26" s="32" t="s">
+        <v>418</v>
+      </c>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
@@ -6903,15 +6901,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>157</v>
+        <v>232</v>
       </c>
       <c r="C27" s="36"/>
-      <c r="D27" s="32" t="s">
-        <v>421</v>
-      </c>
+      <c r="D27" s="36"/>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
@@ -6921,35 +6917,23 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
-        <v>409</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>232</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
+        <v>407</v>
+      </c>
+      <c r="B28" s="93" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="36" t="s">
+        <v>422</v>
+      </c>
+      <c r="D28" s="36" t="s">
+        <v>423</v>
+      </c>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="28" t="s">
-        <v>410</v>
-      </c>
-      <c r="B29" s="93" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6973,9 +6957,8 @@
     <hyperlink ref="A17" r:id="rId13" display="https://drive.google.com/drive/folders/1GhnG5G_BN5lBSXzegcxU-3TuUUTEd6xm" xr:uid="{5F5AAEB7-6B6C-7849-A9BE-EDE531593389}"/>
     <hyperlink ref="A19" r:id="rId14" display="https://drive.google.com/drive/folders/1wcHyiuVUbBeL9ODgyYP-lyy7yM1vMH3u" xr:uid="{C6117B22-7B0A-4D4F-AED4-7357491A8078}"/>
     <hyperlink ref="A21" r:id="rId15" display="https://drive.google.com/drive/folders/1x-FjLa7p2gJDSbRaODzjs8ijaA9SGLtW" xr:uid="{76539FEA-D20F-504F-803D-6634EE2BA126}"/>
-    <hyperlink ref="A22" r:id="rId16" display="https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr" xr:uid="{4C921AD2-E69C-7C40-B1A1-DDA3F76C36D9}"/>
-    <hyperlink ref="A3" r:id="rId17" display="https://drive.google.com/drive/folders/1G8ecO5ODQmn8FX8jzQ962D928BpQ6iUm" xr:uid="{7834EE57-2441-7D43-80AF-2833C3E54227}"/>
-    <hyperlink ref="A23" r:id="rId18" display="https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr" xr:uid="{03D79150-B3F9-F74F-A7DD-3DB4FCCDA7E7}"/>
+    <hyperlink ref="A3" r:id="rId16" display="https://drive.google.com/drive/folders/1G8ecO5ODQmn8FX8jzQ962D928BpQ6iUm" xr:uid="{7834EE57-2441-7D43-80AF-2833C3E54227}"/>
+    <hyperlink ref="A22" r:id="rId17" display="https://drive.google.com/drive/folders/1wMVARUxnYHeiTbbEodCmZFb_vx9FkRVr" xr:uid="{03D79150-B3F9-F74F-A7DD-3DB4FCCDA7E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6999,21 +6982,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="118" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
       <c r="D1" s="82"/>
-      <c r="E1" s="100" t="s">
-        <v>399</v>
-      </c>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="112" t="s">
-        <v>413</v>
-      </c>
-      <c r="I1" s="112"/>
+      <c r="E1" s="108" t="s">
+        <v>397</v>
+      </c>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="120" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1" s="120"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="83" t="s">
@@ -7026,19 +7009,19 @@
         <v>298</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>402</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -7117,7 +7100,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -7169,7 +7152,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7223,7 +7206,7 @@
         <v>25</v>
       </c>
       <c r="H9" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -7250,7 +7233,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -7302,7 +7285,7 @@
         <v>25</v>
       </c>
       <c r="H12" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -7329,7 +7312,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -7356,7 +7339,7 @@
         <v>25</v>
       </c>
       <c r="H14" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -7383,7 +7366,7 @@
         <v>25</v>
       </c>
       <c r="H15" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -7435,7 +7418,7 @@
         <v>25</v>
       </c>
       <c r="H17" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -7512,7 +7495,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -7539,7 +7522,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -7566,7 +7549,7 @@
         <v>25</v>
       </c>
       <c r="H22" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -7593,7 +7576,7 @@
         <v>25</v>
       </c>
       <c r="H23" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -7620,7 +7603,7 @@
         <v>25</v>
       </c>
       <c r="H24" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -7647,7 +7630,7 @@
         <v>25</v>
       </c>
       <c r="H25" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -7674,7 +7657,7 @@
         <v>25</v>
       </c>
       <c r="H26" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -7806,7 +7789,7 @@
         <v>25</v>
       </c>
       <c r="H32" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -7833,7 +7816,7 @@
         <v>25</v>
       </c>
       <c r="H33" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -7937,7 +7920,7 @@
         <v>25</v>
       </c>
       <c r="H37" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -8014,7 +7997,7 @@
         <v>25</v>
       </c>
       <c r="H40" s="74" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -8158,10 +8141,10 @@
         <v>126</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D3" s="70"/>
       <c r="E3" s="70"/>
@@ -8179,7 +8162,7 @@
       <c r="D4" s="70"/>
       <c r="E4" s="70"/>
       <c r="G4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -8189,7 +8172,7 @@
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="64" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B6" s="64" t="s">
         <v>143</v>
@@ -8202,7 +8185,7 @@
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="64" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B7" s="64" t="s">
         <v>144</v>
@@ -8215,7 +8198,7 @@
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B8" s="64" t="s">
         <v>145</v>
@@ -8230,7 +8213,7 @@
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="64" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>147</v>
@@ -8251,7 +8234,7 @@
         <v>148</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="64" t="s">
@@ -8279,7 +8262,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>292</v>
@@ -8296,13 +8279,13 @@
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B17" s="64" t="s">
         <v>305</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="64" t="s">
@@ -8311,13 +8294,13 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="64" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B18" s="64" t="s">
         <v>295</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="64" t="s">
@@ -8331,13 +8314,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="64" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B20" s="64" t="s">
         <v>294</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D20" s="65"/>
       <c r="E20" s="64" t="s">
@@ -8346,13 +8329,13 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="64" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B21" s="64" t="s">
         <v>306</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D21" s="65"/>
       <c r="E21" s="64" t="s">

</xml_diff>

<commit_message>
added Tsys measurment 2B
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AA928F-59FF-8E48-9BD9-D600CCEDA729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D0B7F-41FA-6F4A-B92C-467A4F0C36F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-79460" yWindow="3680" windowWidth="34200" windowHeight="19940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -1434,7 +1434,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1558,6 +1558,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
@@ -1854,7 +1860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2092,6 +2098,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4654,7 +4661,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4844,8 +4851,8 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1WeIiiMAp6TYYdsybsr5MvXeiX_cVX9j0","5C4-004")</f>
         <v>5C4-004</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>169</v>
+      <c r="B6" s="121" t="s">
+        <v>126</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>25</v>
@@ -5430,7 +5437,7 @@
         <v>5C4-019</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>131</v>
@@ -5743,7 +5750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDB6E6A-7294-A941-B453-D346A42E0373}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -6394,7 +6401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9CEE8EE-E616-9C40-8E50-615D9D9C3993}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated feed part inventory
</commit_message>
<xml_diff>
--- a/Antonio-Feed/__FeedPartsInventory.xlsx
+++ b/Antonio-Feed/__FeedPartsInventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D0B7F-41FA-6F4A-B92C-467A4F0C36F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD42A30A-8723-8C4B-BDAF-BB195EB8564D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-79460" yWindow="3680" windowWidth="34200" windowHeight="19940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93320" yWindow="7020" windowWidth="34200" windowHeight="19940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts At ATA" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="433">
   <si>
     <t>Antenna Inventory</t>
   </si>
@@ -1318,6 +1318,30 @@
   </si>
   <si>
     <t xml:space="preserve">3C </t>
+  </si>
+  <si>
+    <t>QRFH V1</t>
+  </si>
+  <si>
+    <t>QRFH V2</t>
+  </si>
+  <si>
+    <t>4270H</t>
+  </si>
+  <si>
+    <t>4332H</t>
+  </si>
+  <si>
+    <t>2287Z</t>
+  </si>
+  <si>
+    <t>2064Z</t>
+  </si>
+  <si>
+    <t>30mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vds=1.20V </t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2059,6 +2083,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2098,7 +2123,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2342,25 +2370,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="109"/>
-      <c r="P1" s="109"/>
-      <c r="Q1" s="109"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="110"/>
+      <c r="P1" s="110"/>
+      <c r="Q1" s="110"/>
     </row>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3672,28 +3700,28 @@
       <c r="A58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="110"/>
-      <c r="B59" s="105"/>
-      <c r="C59" s="105"/>
+      <c r="A59" s="111"/>
+      <c r="B59" s="106"/>
+      <c r="C59" s="106"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="104"/>
-      <c r="B61" s="105"/>
-      <c r="C61" s="104"/>
-      <c r="D61" s="105"/>
-      <c r="E61" s="105"/>
-      <c r="F61" s="105"/>
+      <c r="A61" s="105"/>
+      <c r="B61" s="106"/>
+      <c r="C61" s="105"/>
+      <c r="D61" s="106"/>
+      <c r="E61" s="106"/>
+      <c r="F61" s="106"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="104"/>
-      <c r="B62" s="105"/>
-      <c r="C62" s="104"/>
-      <c r="D62" s="105"/>
-      <c r="E62" s="105"/>
-      <c r="F62" s="105"/>
+      <c r="A62" s="105"/>
+      <c r="B62" s="106"/>
+      <c r="C62" s="105"/>
+      <c r="D62" s="106"/>
+      <c r="E62" s="106"/>
+      <c r="F62" s="106"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4675,20 +4703,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="112" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="113" t="s">
+      <c r="B1" s="113"/>
+      <c r="C1" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
@@ -4851,7 +4879,7 @@
         <f>HYPERLINK("https://drive.google.com/drive/folders/1WeIiiMAp6TYYdsybsr5MvXeiX_cVX9j0","5C4-004")</f>
         <v>5C4-004</v>
       </c>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="104" t="s">
         <v>126</v>
       </c>
       <c r="C6" s="15" t="s">
@@ -5748,10 +5776,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDB6E6A-7294-A941-B453-D346A42E0373}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5760,14 +5788,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="114" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
       <c r="G1" s="62"/>
       <c r="H1" s="62"/>
       <c r="I1" s="62"/>
@@ -6385,6 +6413,40 @@
       </c>
       <c r="F27" s="89" t="s">
         <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="122" t="s">
+        <v>425</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>429</v>
+      </c>
+      <c r="E29" s="123" t="s">
+        <v>431</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="122" t="s">
+        <v>426</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="E30" s="123" t="s">
+        <v>431</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -6413,20 +6475,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="115" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="116" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="116"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="117"/>
     </row>
     <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
@@ -6976,7 +7038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4910D-2B19-014E-928F-E015E5BABD78}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -6989,21 +7051,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="119" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
       <c r="D1" s="82"/>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="109" t="s">
         <v>397</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="120" t="s">
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="121" t="s">
         <v>410</v>
       </c>
-      <c r="I1" s="120"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="83" t="s">

</xml_diff>